<commit_message>
Update 2021 xtabs, add vignette on extra regions
</commit_message>
<xml_diff>
--- a/data-raw/crosstabs/DataHaven2021_Bridgeport_Crosstabs.xlsx
+++ b/data-raw/crosstabs/DataHaven2021_Bridgeport_Crosstabs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarkAbraham\DataHaven Dropbox\2021 Wellbeing Survey\data\Crosstabs\Final Versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0354983-C517-492D-9069-F064EA5C9D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F96113-CD60-4CBF-B18D-C575BAFCF321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="1200" windowWidth="20770" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bridgeport" sheetId="2" r:id="rId1"/>
@@ -213,7 +213,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3264" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3265" uniqueCount="633">
   <si>
     <t>Gender</t>
   </si>
@@ -2110,6 +2110,9 @@
   <si>
     <t>All 5 Cities</t>
   </si>
+  <si>
+    <t>*Note: The survey collects detailed race/ethnicity data, but estimates for all groups are not shown here due to small sample sizes. Refer to DataHaven's Town Equity Reports for more detail.</t>
+  </si>
 </sst>
 </file>
 
@@ -2118,7 +2121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2253,8 +2256,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2434,6 +2454,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -2611,7 +2637,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2672,6 +2698,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2998,7 +3036,7 @@
   <dimension ref="A1:T1929"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1340" sqref="A1340"/>
+      <selection activeCell="A10" sqref="A10:T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3474,26 +3512,28 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
+      <c r="A10" s="23" t="s">
+        <v>632</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="26"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
@@ -70157,279 +70197,896 @@
     </row>
   </sheetData>
   <mergeCells count="1185">
-    <mergeCell ref="A1913:T1913"/>
-    <mergeCell ref="D1914:E1914"/>
-    <mergeCell ref="F1914:I1914"/>
-    <mergeCell ref="J1914:L1914"/>
-    <mergeCell ref="M1914:O1914"/>
-    <mergeCell ref="P1914:R1914"/>
-    <mergeCell ref="S1914:T1914"/>
-    <mergeCell ref="A1895:T1895"/>
-    <mergeCell ref="D1896:E1896"/>
-    <mergeCell ref="F1896:I1896"/>
-    <mergeCell ref="J1896:L1896"/>
-    <mergeCell ref="M1896:O1896"/>
-    <mergeCell ref="P1896:R1896"/>
-    <mergeCell ref="S1896:T1896"/>
-    <mergeCell ref="A1886:T1886"/>
-    <mergeCell ref="D1887:E1887"/>
-    <mergeCell ref="F1887:I1887"/>
-    <mergeCell ref="J1887:L1887"/>
-    <mergeCell ref="M1887:O1887"/>
-    <mergeCell ref="P1887:R1887"/>
-    <mergeCell ref="S1887:T1887"/>
-    <mergeCell ref="A1877:T1877"/>
-    <mergeCell ref="D1878:E1878"/>
-    <mergeCell ref="F1878:I1878"/>
-    <mergeCell ref="J1878:L1878"/>
-    <mergeCell ref="M1878:O1878"/>
-    <mergeCell ref="P1878:R1878"/>
-    <mergeCell ref="S1878:T1878"/>
-    <mergeCell ref="A1868:T1868"/>
-    <mergeCell ref="D1869:E1869"/>
-    <mergeCell ref="F1869:I1869"/>
-    <mergeCell ref="J1869:L1869"/>
-    <mergeCell ref="M1869:O1869"/>
-    <mergeCell ref="P1869:R1869"/>
-    <mergeCell ref="S1869:T1869"/>
-    <mergeCell ref="A1857:T1857"/>
-    <mergeCell ref="D1858:E1858"/>
-    <mergeCell ref="F1858:I1858"/>
-    <mergeCell ref="J1858:L1858"/>
-    <mergeCell ref="M1858:O1858"/>
-    <mergeCell ref="P1858:R1858"/>
-    <mergeCell ref="S1858:T1858"/>
-    <mergeCell ref="A1846:T1846"/>
-    <mergeCell ref="D1847:E1847"/>
-    <mergeCell ref="F1847:I1847"/>
-    <mergeCell ref="J1847:L1847"/>
-    <mergeCell ref="M1847:O1847"/>
-    <mergeCell ref="P1847:R1847"/>
-    <mergeCell ref="S1847:T1847"/>
-    <mergeCell ref="A1834:T1834"/>
-    <mergeCell ref="D1835:E1835"/>
-    <mergeCell ref="F1835:I1835"/>
-    <mergeCell ref="J1835:L1835"/>
-    <mergeCell ref="M1835:O1835"/>
-    <mergeCell ref="P1835:R1835"/>
-    <mergeCell ref="S1835:T1835"/>
-    <mergeCell ref="A1822:T1822"/>
-    <mergeCell ref="D1823:E1823"/>
-    <mergeCell ref="F1823:I1823"/>
-    <mergeCell ref="J1823:L1823"/>
-    <mergeCell ref="M1823:O1823"/>
-    <mergeCell ref="P1823:R1823"/>
-    <mergeCell ref="S1823:T1823"/>
-    <mergeCell ref="A1810:T1810"/>
-    <mergeCell ref="D1811:E1811"/>
-    <mergeCell ref="F1811:I1811"/>
-    <mergeCell ref="J1811:L1811"/>
-    <mergeCell ref="M1811:O1811"/>
-    <mergeCell ref="P1811:R1811"/>
-    <mergeCell ref="S1811:T1811"/>
-    <mergeCell ref="A1798:T1798"/>
-    <mergeCell ref="D1799:E1799"/>
-    <mergeCell ref="F1799:I1799"/>
-    <mergeCell ref="J1799:L1799"/>
-    <mergeCell ref="M1799:O1799"/>
-    <mergeCell ref="P1799:R1799"/>
-    <mergeCell ref="S1799:T1799"/>
-    <mergeCell ref="A1786:T1786"/>
-    <mergeCell ref="D1787:E1787"/>
-    <mergeCell ref="F1787:I1787"/>
-    <mergeCell ref="J1787:L1787"/>
-    <mergeCell ref="M1787:O1787"/>
-    <mergeCell ref="P1787:R1787"/>
-    <mergeCell ref="S1787:T1787"/>
-    <mergeCell ref="A1774:T1774"/>
-    <mergeCell ref="D1775:E1775"/>
-    <mergeCell ref="F1775:I1775"/>
-    <mergeCell ref="J1775:L1775"/>
-    <mergeCell ref="M1775:O1775"/>
-    <mergeCell ref="P1775:R1775"/>
-    <mergeCell ref="S1775:T1775"/>
-    <mergeCell ref="A1762:T1762"/>
-    <mergeCell ref="D1763:E1763"/>
-    <mergeCell ref="F1763:I1763"/>
-    <mergeCell ref="J1763:L1763"/>
-    <mergeCell ref="M1763:O1763"/>
-    <mergeCell ref="P1763:R1763"/>
-    <mergeCell ref="S1763:T1763"/>
-    <mergeCell ref="A1750:T1750"/>
-    <mergeCell ref="D1751:E1751"/>
-    <mergeCell ref="F1751:I1751"/>
-    <mergeCell ref="J1751:L1751"/>
-    <mergeCell ref="M1751:O1751"/>
-    <mergeCell ref="P1751:R1751"/>
-    <mergeCell ref="S1751:T1751"/>
-    <mergeCell ref="A1738:T1738"/>
-    <mergeCell ref="D1739:E1739"/>
-    <mergeCell ref="F1739:I1739"/>
-    <mergeCell ref="J1739:L1739"/>
-    <mergeCell ref="M1739:O1739"/>
-    <mergeCell ref="P1739:R1739"/>
-    <mergeCell ref="S1739:T1739"/>
-    <mergeCell ref="A1726:T1726"/>
-    <mergeCell ref="D1727:E1727"/>
-    <mergeCell ref="F1727:I1727"/>
-    <mergeCell ref="J1727:L1727"/>
-    <mergeCell ref="M1727:O1727"/>
-    <mergeCell ref="P1727:R1727"/>
-    <mergeCell ref="S1727:T1727"/>
-    <mergeCell ref="A1714:T1714"/>
-    <mergeCell ref="D1715:E1715"/>
-    <mergeCell ref="F1715:I1715"/>
-    <mergeCell ref="J1715:L1715"/>
-    <mergeCell ref="M1715:O1715"/>
-    <mergeCell ref="P1715:R1715"/>
-    <mergeCell ref="S1715:T1715"/>
-    <mergeCell ref="A1705:T1705"/>
-    <mergeCell ref="D1706:E1706"/>
-    <mergeCell ref="F1706:I1706"/>
-    <mergeCell ref="J1706:L1706"/>
-    <mergeCell ref="M1706:O1706"/>
-    <mergeCell ref="P1706:R1706"/>
-    <mergeCell ref="S1706:T1706"/>
-    <mergeCell ref="A1693:T1693"/>
-    <mergeCell ref="D1694:E1694"/>
-    <mergeCell ref="F1694:I1694"/>
-    <mergeCell ref="J1694:L1694"/>
-    <mergeCell ref="M1694:O1694"/>
-    <mergeCell ref="P1694:R1694"/>
-    <mergeCell ref="S1694:T1694"/>
-    <mergeCell ref="A1683:T1683"/>
-    <mergeCell ref="D1684:E1684"/>
-    <mergeCell ref="F1684:I1684"/>
-    <mergeCell ref="J1684:L1684"/>
-    <mergeCell ref="M1684:O1684"/>
-    <mergeCell ref="P1684:R1684"/>
-    <mergeCell ref="S1684:T1684"/>
-    <mergeCell ref="A1674:T1674"/>
-    <mergeCell ref="D1675:E1675"/>
-    <mergeCell ref="F1675:I1675"/>
-    <mergeCell ref="J1675:L1675"/>
-    <mergeCell ref="M1675:O1675"/>
-    <mergeCell ref="P1675:R1675"/>
-    <mergeCell ref="S1675:T1675"/>
-    <mergeCell ref="A1662:T1662"/>
-    <mergeCell ref="D1663:E1663"/>
-    <mergeCell ref="F1663:I1663"/>
-    <mergeCell ref="J1663:L1663"/>
-    <mergeCell ref="M1663:O1663"/>
-    <mergeCell ref="P1663:R1663"/>
-    <mergeCell ref="S1663:T1663"/>
-    <mergeCell ref="A1652:T1652"/>
-    <mergeCell ref="D1653:E1653"/>
-    <mergeCell ref="F1653:I1653"/>
-    <mergeCell ref="J1653:L1653"/>
-    <mergeCell ref="M1653:O1653"/>
-    <mergeCell ref="P1653:R1653"/>
-    <mergeCell ref="S1653:T1653"/>
-    <mergeCell ref="A1642:T1642"/>
-    <mergeCell ref="D1643:E1643"/>
-    <mergeCell ref="F1643:I1643"/>
-    <mergeCell ref="J1643:L1643"/>
-    <mergeCell ref="M1643:O1643"/>
-    <mergeCell ref="P1643:R1643"/>
-    <mergeCell ref="S1643:T1643"/>
-    <mergeCell ref="A1632:T1632"/>
-    <mergeCell ref="D1633:E1633"/>
-    <mergeCell ref="F1633:I1633"/>
-    <mergeCell ref="J1633:L1633"/>
-    <mergeCell ref="M1633:O1633"/>
-    <mergeCell ref="P1633:R1633"/>
-    <mergeCell ref="S1633:T1633"/>
-    <mergeCell ref="A1619:T1619"/>
-    <mergeCell ref="D1620:E1620"/>
-    <mergeCell ref="F1620:I1620"/>
-    <mergeCell ref="J1620:L1620"/>
-    <mergeCell ref="M1620:O1620"/>
-    <mergeCell ref="P1620:R1620"/>
-    <mergeCell ref="S1620:T1620"/>
-    <mergeCell ref="A1601:T1601"/>
-    <mergeCell ref="D1602:E1602"/>
-    <mergeCell ref="F1602:I1602"/>
-    <mergeCell ref="J1602:L1602"/>
-    <mergeCell ref="M1602:O1602"/>
-    <mergeCell ref="P1602:R1602"/>
-    <mergeCell ref="S1602:T1602"/>
-    <mergeCell ref="A1589:T1589"/>
-    <mergeCell ref="D1590:E1590"/>
-    <mergeCell ref="F1590:I1590"/>
-    <mergeCell ref="J1590:L1590"/>
-    <mergeCell ref="M1590:O1590"/>
-    <mergeCell ref="P1590:R1590"/>
-    <mergeCell ref="S1590:T1590"/>
-    <mergeCell ref="A1580:T1580"/>
-    <mergeCell ref="D1581:E1581"/>
-    <mergeCell ref="F1581:I1581"/>
-    <mergeCell ref="J1581:L1581"/>
-    <mergeCell ref="M1581:O1581"/>
-    <mergeCell ref="P1581:R1581"/>
-    <mergeCell ref="S1581:T1581"/>
-    <mergeCell ref="A1568:T1568"/>
-    <mergeCell ref="D1569:E1569"/>
-    <mergeCell ref="F1569:I1569"/>
-    <mergeCell ref="J1569:L1569"/>
-    <mergeCell ref="M1569:O1569"/>
-    <mergeCell ref="P1569:R1569"/>
-    <mergeCell ref="S1569:T1569"/>
-    <mergeCell ref="A1559:T1559"/>
-    <mergeCell ref="D1560:E1560"/>
-    <mergeCell ref="F1560:I1560"/>
-    <mergeCell ref="J1560:L1560"/>
-    <mergeCell ref="M1560:O1560"/>
-    <mergeCell ref="P1560:R1560"/>
-    <mergeCell ref="S1560:T1560"/>
-    <mergeCell ref="A1550:T1550"/>
-    <mergeCell ref="D1551:E1551"/>
-    <mergeCell ref="F1551:I1551"/>
-    <mergeCell ref="J1551:L1551"/>
-    <mergeCell ref="M1551:O1551"/>
-    <mergeCell ref="P1551:R1551"/>
-    <mergeCell ref="S1551:T1551"/>
-    <mergeCell ref="A1541:T1541"/>
-    <mergeCell ref="D1542:E1542"/>
-    <mergeCell ref="F1542:I1542"/>
-    <mergeCell ref="J1542:L1542"/>
-    <mergeCell ref="M1542:O1542"/>
-    <mergeCell ref="P1542:R1542"/>
-    <mergeCell ref="S1542:T1542"/>
-    <mergeCell ref="A1531:T1531"/>
-    <mergeCell ref="D1532:E1532"/>
-    <mergeCell ref="F1532:I1532"/>
-    <mergeCell ref="J1532:L1532"/>
-    <mergeCell ref="M1532:O1532"/>
-    <mergeCell ref="P1532:R1532"/>
-    <mergeCell ref="S1532:T1532"/>
-    <mergeCell ref="A1521:T1521"/>
-    <mergeCell ref="D1522:E1522"/>
-    <mergeCell ref="F1522:I1522"/>
-    <mergeCell ref="J1522:L1522"/>
-    <mergeCell ref="M1522:O1522"/>
-    <mergeCell ref="P1522:R1522"/>
-    <mergeCell ref="S1522:T1522"/>
-    <mergeCell ref="A1511:T1511"/>
-    <mergeCell ref="D1512:E1512"/>
-    <mergeCell ref="F1512:I1512"/>
-    <mergeCell ref="J1512:L1512"/>
-    <mergeCell ref="M1512:O1512"/>
-    <mergeCell ref="P1512:R1512"/>
-    <mergeCell ref="S1512:T1512"/>
-    <mergeCell ref="A1501:T1501"/>
-    <mergeCell ref="D1502:E1502"/>
-    <mergeCell ref="F1502:I1502"/>
-    <mergeCell ref="J1502:L1502"/>
-    <mergeCell ref="M1502:O1502"/>
-    <mergeCell ref="P1502:R1502"/>
-    <mergeCell ref="S1502:T1502"/>
-    <mergeCell ref="A1491:T1491"/>
-    <mergeCell ref="D1492:E1492"/>
-    <mergeCell ref="F1492:I1492"/>
-    <mergeCell ref="J1492:L1492"/>
-    <mergeCell ref="M1492:O1492"/>
-    <mergeCell ref="P1492:R1492"/>
-    <mergeCell ref="S1492:T1492"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="A25:T25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="A24:T24"/>
+    <mergeCell ref="A11:T11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="A61:T61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="J62:L62"/>
+    <mergeCell ref="M62:O62"/>
+    <mergeCell ref="P62:R62"/>
+    <mergeCell ref="S62:T62"/>
+    <mergeCell ref="A49:T49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="J50:L50"/>
+    <mergeCell ref="M50:O50"/>
+    <mergeCell ref="P50:R50"/>
+    <mergeCell ref="S50:T50"/>
+    <mergeCell ref="A37:T37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="P38:R38"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="A97:T97"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="J98:L98"/>
+    <mergeCell ref="M98:O98"/>
+    <mergeCell ref="P98:R98"/>
+    <mergeCell ref="S98:T98"/>
+    <mergeCell ref="A85:T85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="F86:I86"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M86:O86"/>
+    <mergeCell ref="P86:R86"/>
+    <mergeCell ref="S86:T86"/>
+    <mergeCell ref="A73:T73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="F74:I74"/>
+    <mergeCell ref="J74:L74"/>
+    <mergeCell ref="M74:O74"/>
+    <mergeCell ref="P74:R74"/>
+    <mergeCell ref="S74:T74"/>
+    <mergeCell ref="A133:T133"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="F134:I134"/>
+    <mergeCell ref="J134:L134"/>
+    <mergeCell ref="M134:O134"/>
+    <mergeCell ref="P134:R134"/>
+    <mergeCell ref="S134:T134"/>
+    <mergeCell ref="A121:T121"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="F122:I122"/>
+    <mergeCell ref="J122:L122"/>
+    <mergeCell ref="M122:O122"/>
+    <mergeCell ref="P122:R122"/>
+    <mergeCell ref="S122:T122"/>
+    <mergeCell ref="A109:T109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="F110:I110"/>
+    <mergeCell ref="J110:L110"/>
+    <mergeCell ref="M110:O110"/>
+    <mergeCell ref="P110:R110"/>
+    <mergeCell ref="S110:T110"/>
+    <mergeCell ref="A169:T169"/>
+    <mergeCell ref="D170:E170"/>
+    <mergeCell ref="F170:I170"/>
+    <mergeCell ref="J170:L170"/>
+    <mergeCell ref="M170:O170"/>
+    <mergeCell ref="P170:R170"/>
+    <mergeCell ref="S170:T170"/>
+    <mergeCell ref="A157:T157"/>
+    <mergeCell ref="D158:E158"/>
+    <mergeCell ref="F158:I158"/>
+    <mergeCell ref="J158:L158"/>
+    <mergeCell ref="M158:O158"/>
+    <mergeCell ref="P158:R158"/>
+    <mergeCell ref="S158:T158"/>
+    <mergeCell ref="A145:T145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="F146:I146"/>
+    <mergeCell ref="J146:L146"/>
+    <mergeCell ref="M146:O146"/>
+    <mergeCell ref="P146:R146"/>
+    <mergeCell ref="S146:T146"/>
+    <mergeCell ref="A206:T206"/>
+    <mergeCell ref="D207:E207"/>
+    <mergeCell ref="F207:I207"/>
+    <mergeCell ref="J207:L207"/>
+    <mergeCell ref="M207:O207"/>
+    <mergeCell ref="P207:R207"/>
+    <mergeCell ref="S207:T207"/>
+    <mergeCell ref="A195:T195"/>
+    <mergeCell ref="D196:E196"/>
+    <mergeCell ref="F196:I196"/>
+    <mergeCell ref="J196:L196"/>
+    <mergeCell ref="M196:O196"/>
+    <mergeCell ref="P196:R196"/>
+    <mergeCell ref="S196:T196"/>
+    <mergeCell ref="A182:T182"/>
+    <mergeCell ref="D183:E183"/>
+    <mergeCell ref="F183:I183"/>
+    <mergeCell ref="J183:L183"/>
+    <mergeCell ref="M183:O183"/>
+    <mergeCell ref="P183:R183"/>
+    <mergeCell ref="S183:T183"/>
+    <mergeCell ref="A253:T253"/>
+    <mergeCell ref="A239:T239"/>
+    <mergeCell ref="D240:E240"/>
+    <mergeCell ref="F240:I240"/>
+    <mergeCell ref="J240:L240"/>
+    <mergeCell ref="M240:O240"/>
+    <mergeCell ref="P240:R240"/>
+    <mergeCell ref="S240:T240"/>
+    <mergeCell ref="A229:T229"/>
+    <mergeCell ref="D230:E230"/>
+    <mergeCell ref="F230:I230"/>
+    <mergeCell ref="J230:L230"/>
+    <mergeCell ref="M230:O230"/>
+    <mergeCell ref="P230:R230"/>
+    <mergeCell ref="S230:T230"/>
+    <mergeCell ref="A219:T219"/>
+    <mergeCell ref="D220:E220"/>
+    <mergeCell ref="F220:I220"/>
+    <mergeCell ref="J220:L220"/>
+    <mergeCell ref="M220:O220"/>
+    <mergeCell ref="P220:R220"/>
+    <mergeCell ref="S220:T220"/>
+    <mergeCell ref="A278:T278"/>
+    <mergeCell ref="D279:E279"/>
+    <mergeCell ref="F279:I279"/>
+    <mergeCell ref="J279:L279"/>
+    <mergeCell ref="M279:O279"/>
+    <mergeCell ref="P279:R279"/>
+    <mergeCell ref="S279:T279"/>
+    <mergeCell ref="A266:T266"/>
+    <mergeCell ref="D267:E267"/>
+    <mergeCell ref="F267:I267"/>
+    <mergeCell ref="J267:L267"/>
+    <mergeCell ref="M267:O267"/>
+    <mergeCell ref="P267:R267"/>
+    <mergeCell ref="S267:T267"/>
+    <mergeCell ref="A254:T254"/>
+    <mergeCell ref="D255:E255"/>
+    <mergeCell ref="F255:I255"/>
+    <mergeCell ref="J255:L255"/>
+    <mergeCell ref="M255:O255"/>
+    <mergeCell ref="P255:R255"/>
+    <mergeCell ref="S255:T255"/>
+    <mergeCell ref="A315:T315"/>
+    <mergeCell ref="D316:E316"/>
+    <mergeCell ref="F316:I316"/>
+    <mergeCell ref="J316:L316"/>
+    <mergeCell ref="M316:O316"/>
+    <mergeCell ref="P316:R316"/>
+    <mergeCell ref="S316:T316"/>
+    <mergeCell ref="A314:T314"/>
+    <mergeCell ref="A302:T302"/>
+    <mergeCell ref="D303:E303"/>
+    <mergeCell ref="F303:I303"/>
+    <mergeCell ref="J303:L303"/>
+    <mergeCell ref="M303:O303"/>
+    <mergeCell ref="P303:R303"/>
+    <mergeCell ref="S303:T303"/>
+    <mergeCell ref="A290:T290"/>
+    <mergeCell ref="D291:E291"/>
+    <mergeCell ref="F291:I291"/>
+    <mergeCell ref="J291:L291"/>
+    <mergeCell ref="M291:O291"/>
+    <mergeCell ref="P291:R291"/>
+    <mergeCell ref="S291:T291"/>
+    <mergeCell ref="A354:T354"/>
+    <mergeCell ref="D355:E355"/>
+    <mergeCell ref="F355:I355"/>
+    <mergeCell ref="J355:L355"/>
+    <mergeCell ref="M355:O355"/>
+    <mergeCell ref="P355:R355"/>
+    <mergeCell ref="S355:T355"/>
+    <mergeCell ref="A341:T341"/>
+    <mergeCell ref="D342:E342"/>
+    <mergeCell ref="F342:I342"/>
+    <mergeCell ref="J342:L342"/>
+    <mergeCell ref="M342:O342"/>
+    <mergeCell ref="P342:R342"/>
+    <mergeCell ref="S342:T342"/>
+    <mergeCell ref="A328:T328"/>
+    <mergeCell ref="D329:E329"/>
+    <mergeCell ref="F329:I329"/>
+    <mergeCell ref="J329:L329"/>
+    <mergeCell ref="M329:O329"/>
+    <mergeCell ref="P329:R329"/>
+    <mergeCell ref="S329:T329"/>
+    <mergeCell ref="A390:T390"/>
+    <mergeCell ref="D391:E391"/>
+    <mergeCell ref="F391:I391"/>
+    <mergeCell ref="J391:L391"/>
+    <mergeCell ref="M391:O391"/>
+    <mergeCell ref="P391:R391"/>
+    <mergeCell ref="S391:T391"/>
+    <mergeCell ref="A380:T380"/>
+    <mergeCell ref="D381:E381"/>
+    <mergeCell ref="F381:I381"/>
+    <mergeCell ref="J381:L381"/>
+    <mergeCell ref="M381:O381"/>
+    <mergeCell ref="P381:R381"/>
+    <mergeCell ref="S381:T381"/>
+    <mergeCell ref="A367:T367"/>
+    <mergeCell ref="D368:E368"/>
+    <mergeCell ref="F368:I368"/>
+    <mergeCell ref="J368:L368"/>
+    <mergeCell ref="M368:O368"/>
+    <mergeCell ref="P368:R368"/>
+    <mergeCell ref="S368:T368"/>
+    <mergeCell ref="A423:T423"/>
+    <mergeCell ref="D424:E424"/>
+    <mergeCell ref="F424:I424"/>
+    <mergeCell ref="J424:L424"/>
+    <mergeCell ref="M424:O424"/>
+    <mergeCell ref="P424:R424"/>
+    <mergeCell ref="S424:T424"/>
+    <mergeCell ref="A410:T410"/>
+    <mergeCell ref="D411:E411"/>
+    <mergeCell ref="F411:I411"/>
+    <mergeCell ref="J411:L411"/>
+    <mergeCell ref="M411:O411"/>
+    <mergeCell ref="P411:R411"/>
+    <mergeCell ref="S411:T411"/>
+    <mergeCell ref="A400:T400"/>
+    <mergeCell ref="D401:E401"/>
+    <mergeCell ref="F401:I401"/>
+    <mergeCell ref="J401:L401"/>
+    <mergeCell ref="M401:O401"/>
+    <mergeCell ref="P401:R401"/>
+    <mergeCell ref="S401:T401"/>
+    <mergeCell ref="A462:T462"/>
+    <mergeCell ref="D463:E463"/>
+    <mergeCell ref="F463:I463"/>
+    <mergeCell ref="J463:L463"/>
+    <mergeCell ref="M463:O463"/>
+    <mergeCell ref="P463:R463"/>
+    <mergeCell ref="S463:T463"/>
+    <mergeCell ref="A449:T449"/>
+    <mergeCell ref="D450:E450"/>
+    <mergeCell ref="F450:I450"/>
+    <mergeCell ref="J450:L450"/>
+    <mergeCell ref="M450:O450"/>
+    <mergeCell ref="P450:R450"/>
+    <mergeCell ref="S450:T450"/>
+    <mergeCell ref="A436:T436"/>
+    <mergeCell ref="D437:E437"/>
+    <mergeCell ref="F437:I437"/>
+    <mergeCell ref="J437:L437"/>
+    <mergeCell ref="M437:O437"/>
+    <mergeCell ref="P437:R437"/>
+    <mergeCell ref="S437:T437"/>
+    <mergeCell ref="A501:T501"/>
+    <mergeCell ref="D502:E502"/>
+    <mergeCell ref="F502:I502"/>
+    <mergeCell ref="J502:L502"/>
+    <mergeCell ref="M502:O502"/>
+    <mergeCell ref="P502:R502"/>
+    <mergeCell ref="S502:T502"/>
+    <mergeCell ref="A491:T491"/>
+    <mergeCell ref="D492:E492"/>
+    <mergeCell ref="F492:I492"/>
+    <mergeCell ref="J492:L492"/>
+    <mergeCell ref="M492:O492"/>
+    <mergeCell ref="P492:R492"/>
+    <mergeCell ref="S492:T492"/>
+    <mergeCell ref="A490:T490"/>
+    <mergeCell ref="A475:T475"/>
+    <mergeCell ref="D476:E476"/>
+    <mergeCell ref="F476:I476"/>
+    <mergeCell ref="J476:L476"/>
+    <mergeCell ref="M476:O476"/>
+    <mergeCell ref="P476:R476"/>
+    <mergeCell ref="S476:T476"/>
+    <mergeCell ref="A536:T536"/>
+    <mergeCell ref="D537:E537"/>
+    <mergeCell ref="F537:I537"/>
+    <mergeCell ref="J537:L537"/>
+    <mergeCell ref="M537:O537"/>
+    <mergeCell ref="P537:R537"/>
+    <mergeCell ref="S537:T537"/>
+    <mergeCell ref="A526:T526"/>
+    <mergeCell ref="D527:E527"/>
+    <mergeCell ref="F527:I527"/>
+    <mergeCell ref="J527:L527"/>
+    <mergeCell ref="M527:O527"/>
+    <mergeCell ref="P527:R527"/>
+    <mergeCell ref="S527:T527"/>
+    <mergeCell ref="A511:T511"/>
+    <mergeCell ref="D512:E512"/>
+    <mergeCell ref="F512:I512"/>
+    <mergeCell ref="J512:L512"/>
+    <mergeCell ref="M512:O512"/>
+    <mergeCell ref="P512:R512"/>
+    <mergeCell ref="S512:T512"/>
+    <mergeCell ref="A572:T572"/>
+    <mergeCell ref="D573:E573"/>
+    <mergeCell ref="F573:I573"/>
+    <mergeCell ref="J573:L573"/>
+    <mergeCell ref="M573:O573"/>
+    <mergeCell ref="P573:R573"/>
+    <mergeCell ref="S573:T573"/>
+    <mergeCell ref="A558:T558"/>
+    <mergeCell ref="D559:E559"/>
+    <mergeCell ref="F559:I559"/>
+    <mergeCell ref="J559:L559"/>
+    <mergeCell ref="M559:O559"/>
+    <mergeCell ref="P559:R559"/>
+    <mergeCell ref="S559:T559"/>
+    <mergeCell ref="A546:T546"/>
+    <mergeCell ref="D547:E547"/>
+    <mergeCell ref="F547:I547"/>
+    <mergeCell ref="J547:L547"/>
+    <mergeCell ref="M547:O547"/>
+    <mergeCell ref="P547:R547"/>
+    <mergeCell ref="S547:T547"/>
+    <mergeCell ref="A606:T606"/>
+    <mergeCell ref="D607:E607"/>
+    <mergeCell ref="F607:I607"/>
+    <mergeCell ref="J607:L607"/>
+    <mergeCell ref="M607:O607"/>
+    <mergeCell ref="P607:R607"/>
+    <mergeCell ref="S607:T607"/>
+    <mergeCell ref="A592:T592"/>
+    <mergeCell ref="D593:E593"/>
+    <mergeCell ref="F593:I593"/>
+    <mergeCell ref="J593:L593"/>
+    <mergeCell ref="M593:O593"/>
+    <mergeCell ref="P593:R593"/>
+    <mergeCell ref="S593:T593"/>
+    <mergeCell ref="A582:T582"/>
+    <mergeCell ref="D583:E583"/>
+    <mergeCell ref="F583:I583"/>
+    <mergeCell ref="J583:L583"/>
+    <mergeCell ref="M583:O583"/>
+    <mergeCell ref="P583:R583"/>
+    <mergeCell ref="S583:T583"/>
+    <mergeCell ref="A637:T637"/>
+    <mergeCell ref="D638:E638"/>
+    <mergeCell ref="F638:I638"/>
+    <mergeCell ref="J638:L638"/>
+    <mergeCell ref="M638:O638"/>
+    <mergeCell ref="P638:R638"/>
+    <mergeCell ref="S638:T638"/>
+    <mergeCell ref="A627:T627"/>
+    <mergeCell ref="D628:E628"/>
+    <mergeCell ref="F628:I628"/>
+    <mergeCell ref="J628:L628"/>
+    <mergeCell ref="M628:O628"/>
+    <mergeCell ref="P628:R628"/>
+    <mergeCell ref="S628:T628"/>
+    <mergeCell ref="A626:T626"/>
+    <mergeCell ref="A616:T616"/>
+    <mergeCell ref="D617:E617"/>
+    <mergeCell ref="F617:I617"/>
+    <mergeCell ref="J617:L617"/>
+    <mergeCell ref="M617:O617"/>
+    <mergeCell ref="P617:R617"/>
+    <mergeCell ref="S617:T617"/>
+    <mergeCell ref="A667:T667"/>
+    <mergeCell ref="D668:E668"/>
+    <mergeCell ref="F668:I668"/>
+    <mergeCell ref="J668:L668"/>
+    <mergeCell ref="M668:O668"/>
+    <mergeCell ref="P668:R668"/>
+    <mergeCell ref="S668:T668"/>
+    <mergeCell ref="A657:T657"/>
+    <mergeCell ref="D658:E658"/>
+    <mergeCell ref="F658:I658"/>
+    <mergeCell ref="J658:L658"/>
+    <mergeCell ref="M658:O658"/>
+    <mergeCell ref="P658:R658"/>
+    <mergeCell ref="S658:T658"/>
+    <mergeCell ref="A647:T647"/>
+    <mergeCell ref="D648:E648"/>
+    <mergeCell ref="F648:I648"/>
+    <mergeCell ref="J648:L648"/>
+    <mergeCell ref="M648:O648"/>
+    <mergeCell ref="P648:R648"/>
+    <mergeCell ref="S648:T648"/>
+    <mergeCell ref="A697:T697"/>
+    <mergeCell ref="D698:E698"/>
+    <mergeCell ref="F698:I698"/>
+    <mergeCell ref="J698:L698"/>
+    <mergeCell ref="M698:O698"/>
+    <mergeCell ref="P698:R698"/>
+    <mergeCell ref="S698:T698"/>
+    <mergeCell ref="A687:T687"/>
+    <mergeCell ref="D688:E688"/>
+    <mergeCell ref="F688:I688"/>
+    <mergeCell ref="J688:L688"/>
+    <mergeCell ref="M688:O688"/>
+    <mergeCell ref="P688:R688"/>
+    <mergeCell ref="S688:T688"/>
+    <mergeCell ref="A677:T677"/>
+    <mergeCell ref="D678:E678"/>
+    <mergeCell ref="F678:I678"/>
+    <mergeCell ref="J678:L678"/>
+    <mergeCell ref="M678:O678"/>
+    <mergeCell ref="P678:R678"/>
+    <mergeCell ref="S678:T678"/>
+    <mergeCell ref="A727:T727"/>
+    <mergeCell ref="D728:E728"/>
+    <mergeCell ref="F728:I728"/>
+    <mergeCell ref="J728:L728"/>
+    <mergeCell ref="M728:O728"/>
+    <mergeCell ref="P728:R728"/>
+    <mergeCell ref="S728:T728"/>
+    <mergeCell ref="A717:T717"/>
+    <mergeCell ref="D718:E718"/>
+    <mergeCell ref="F718:I718"/>
+    <mergeCell ref="J718:L718"/>
+    <mergeCell ref="M718:O718"/>
+    <mergeCell ref="P718:R718"/>
+    <mergeCell ref="S718:T718"/>
+    <mergeCell ref="A707:T707"/>
+    <mergeCell ref="D708:E708"/>
+    <mergeCell ref="F708:I708"/>
+    <mergeCell ref="J708:L708"/>
+    <mergeCell ref="M708:O708"/>
+    <mergeCell ref="P708:R708"/>
+    <mergeCell ref="S708:T708"/>
+    <mergeCell ref="A759:T759"/>
+    <mergeCell ref="D760:E760"/>
+    <mergeCell ref="F760:I760"/>
+    <mergeCell ref="J760:L760"/>
+    <mergeCell ref="M760:O760"/>
+    <mergeCell ref="P760:R760"/>
+    <mergeCell ref="S760:T760"/>
+    <mergeCell ref="A749:T749"/>
+    <mergeCell ref="D750:E750"/>
+    <mergeCell ref="F750:I750"/>
+    <mergeCell ref="J750:L750"/>
+    <mergeCell ref="M750:O750"/>
+    <mergeCell ref="P750:R750"/>
+    <mergeCell ref="S750:T750"/>
+    <mergeCell ref="A739:T739"/>
+    <mergeCell ref="D740:E740"/>
+    <mergeCell ref="F740:I740"/>
+    <mergeCell ref="J740:L740"/>
+    <mergeCell ref="M740:O740"/>
+    <mergeCell ref="P740:R740"/>
+    <mergeCell ref="S740:T740"/>
+    <mergeCell ref="A792:T792"/>
+    <mergeCell ref="D793:E793"/>
+    <mergeCell ref="F793:I793"/>
+    <mergeCell ref="J793:L793"/>
+    <mergeCell ref="M793:O793"/>
+    <mergeCell ref="P793:R793"/>
+    <mergeCell ref="S793:T793"/>
+    <mergeCell ref="A781:T781"/>
+    <mergeCell ref="D782:E782"/>
+    <mergeCell ref="F782:I782"/>
+    <mergeCell ref="J782:L782"/>
+    <mergeCell ref="M782:O782"/>
+    <mergeCell ref="P782:R782"/>
+    <mergeCell ref="S782:T782"/>
+    <mergeCell ref="A770:T770"/>
+    <mergeCell ref="D771:E771"/>
+    <mergeCell ref="F771:I771"/>
+    <mergeCell ref="J771:L771"/>
+    <mergeCell ref="M771:O771"/>
+    <mergeCell ref="P771:R771"/>
+    <mergeCell ref="S771:T771"/>
+    <mergeCell ref="A831:T831"/>
+    <mergeCell ref="D832:E832"/>
+    <mergeCell ref="F832:I832"/>
+    <mergeCell ref="J832:L832"/>
+    <mergeCell ref="M832:O832"/>
+    <mergeCell ref="P832:R832"/>
+    <mergeCell ref="S832:T832"/>
+    <mergeCell ref="A819:T819"/>
+    <mergeCell ref="D820:E820"/>
+    <mergeCell ref="F820:I820"/>
+    <mergeCell ref="J820:L820"/>
+    <mergeCell ref="M820:O820"/>
+    <mergeCell ref="P820:R820"/>
+    <mergeCell ref="S820:T820"/>
+    <mergeCell ref="A818:T818"/>
+    <mergeCell ref="A805:T805"/>
+    <mergeCell ref="D806:E806"/>
+    <mergeCell ref="F806:I806"/>
+    <mergeCell ref="J806:L806"/>
+    <mergeCell ref="M806:O806"/>
+    <mergeCell ref="P806:R806"/>
+    <mergeCell ref="S806:T806"/>
+    <mergeCell ref="A870:T870"/>
+    <mergeCell ref="D871:E871"/>
+    <mergeCell ref="F871:I871"/>
+    <mergeCell ref="J871:L871"/>
+    <mergeCell ref="M871:O871"/>
+    <mergeCell ref="P871:R871"/>
+    <mergeCell ref="S871:T871"/>
+    <mergeCell ref="A860:T860"/>
+    <mergeCell ref="D861:E861"/>
+    <mergeCell ref="F861:I861"/>
+    <mergeCell ref="J861:L861"/>
+    <mergeCell ref="M861:O861"/>
+    <mergeCell ref="P861:R861"/>
+    <mergeCell ref="S861:T861"/>
+    <mergeCell ref="A843:T843"/>
+    <mergeCell ref="D844:E844"/>
+    <mergeCell ref="F844:I844"/>
+    <mergeCell ref="J844:L844"/>
+    <mergeCell ref="M844:O844"/>
+    <mergeCell ref="P844:R844"/>
+    <mergeCell ref="S844:T844"/>
+    <mergeCell ref="A904:T904"/>
+    <mergeCell ref="D905:E905"/>
+    <mergeCell ref="F905:I905"/>
+    <mergeCell ref="J905:L905"/>
+    <mergeCell ref="M905:O905"/>
+    <mergeCell ref="P905:R905"/>
+    <mergeCell ref="S905:T905"/>
+    <mergeCell ref="A892:T892"/>
+    <mergeCell ref="D893:E893"/>
+    <mergeCell ref="F893:I893"/>
+    <mergeCell ref="J893:L893"/>
+    <mergeCell ref="M893:O893"/>
+    <mergeCell ref="P893:R893"/>
+    <mergeCell ref="S893:T893"/>
+    <mergeCell ref="A882:T882"/>
+    <mergeCell ref="D883:E883"/>
+    <mergeCell ref="F883:I883"/>
+    <mergeCell ref="J883:L883"/>
+    <mergeCell ref="M883:O883"/>
+    <mergeCell ref="P883:R883"/>
+    <mergeCell ref="S883:T883"/>
+    <mergeCell ref="A939:T939"/>
+    <mergeCell ref="D940:E940"/>
+    <mergeCell ref="F940:I940"/>
+    <mergeCell ref="J940:L940"/>
+    <mergeCell ref="M940:O940"/>
+    <mergeCell ref="P940:R940"/>
+    <mergeCell ref="S940:T940"/>
+    <mergeCell ref="A928:T928"/>
+    <mergeCell ref="D929:E929"/>
+    <mergeCell ref="F929:I929"/>
+    <mergeCell ref="J929:L929"/>
+    <mergeCell ref="M929:O929"/>
+    <mergeCell ref="P929:R929"/>
+    <mergeCell ref="S929:T929"/>
+    <mergeCell ref="A916:T916"/>
+    <mergeCell ref="D917:E917"/>
+    <mergeCell ref="F917:I917"/>
+    <mergeCell ref="J917:L917"/>
+    <mergeCell ref="M917:O917"/>
+    <mergeCell ref="P917:R917"/>
+    <mergeCell ref="S917:T917"/>
+    <mergeCell ref="A971:T971"/>
+    <mergeCell ref="D972:E972"/>
+    <mergeCell ref="F972:I972"/>
+    <mergeCell ref="J972:L972"/>
+    <mergeCell ref="M972:O972"/>
+    <mergeCell ref="P972:R972"/>
+    <mergeCell ref="S972:T972"/>
+    <mergeCell ref="A959:T959"/>
+    <mergeCell ref="D960:E960"/>
+    <mergeCell ref="F960:I960"/>
+    <mergeCell ref="J960:L960"/>
+    <mergeCell ref="M960:O960"/>
+    <mergeCell ref="P960:R960"/>
+    <mergeCell ref="S960:T960"/>
+    <mergeCell ref="A949:T949"/>
+    <mergeCell ref="D950:E950"/>
+    <mergeCell ref="F950:I950"/>
+    <mergeCell ref="J950:L950"/>
+    <mergeCell ref="M950:O950"/>
+    <mergeCell ref="P950:R950"/>
+    <mergeCell ref="S950:T950"/>
+    <mergeCell ref="A1006:T1006"/>
+    <mergeCell ref="D1007:E1007"/>
+    <mergeCell ref="F1007:I1007"/>
+    <mergeCell ref="J1007:L1007"/>
+    <mergeCell ref="M1007:O1007"/>
+    <mergeCell ref="P1007:R1007"/>
+    <mergeCell ref="S1007:T1007"/>
+    <mergeCell ref="A995:T995"/>
+    <mergeCell ref="D996:E996"/>
+    <mergeCell ref="F996:I996"/>
+    <mergeCell ref="J996:L996"/>
+    <mergeCell ref="M996:O996"/>
+    <mergeCell ref="P996:R996"/>
+    <mergeCell ref="S996:T996"/>
+    <mergeCell ref="A984:T984"/>
+    <mergeCell ref="D985:E985"/>
+    <mergeCell ref="F985:I985"/>
+    <mergeCell ref="J985:L985"/>
+    <mergeCell ref="M985:O985"/>
+    <mergeCell ref="P985:R985"/>
+    <mergeCell ref="S985:T985"/>
+    <mergeCell ref="A1041:T1041"/>
+    <mergeCell ref="D1042:E1042"/>
+    <mergeCell ref="F1042:I1042"/>
+    <mergeCell ref="J1042:L1042"/>
+    <mergeCell ref="M1042:O1042"/>
+    <mergeCell ref="P1042:R1042"/>
+    <mergeCell ref="S1042:T1042"/>
+    <mergeCell ref="A1031:T1031"/>
+    <mergeCell ref="D1032:E1032"/>
+    <mergeCell ref="F1032:I1032"/>
+    <mergeCell ref="J1032:L1032"/>
+    <mergeCell ref="M1032:O1032"/>
+    <mergeCell ref="P1032:R1032"/>
+    <mergeCell ref="S1032:T1032"/>
+    <mergeCell ref="A1017:T1017"/>
+    <mergeCell ref="D1018:E1018"/>
+    <mergeCell ref="F1018:I1018"/>
+    <mergeCell ref="J1018:L1018"/>
+    <mergeCell ref="M1018:O1018"/>
+    <mergeCell ref="P1018:R1018"/>
+    <mergeCell ref="S1018:T1018"/>
+    <mergeCell ref="A1076:T1076"/>
+    <mergeCell ref="D1077:E1077"/>
+    <mergeCell ref="F1077:I1077"/>
+    <mergeCell ref="J1077:L1077"/>
+    <mergeCell ref="M1077:O1077"/>
+    <mergeCell ref="P1077:R1077"/>
+    <mergeCell ref="S1077:T1077"/>
+    <mergeCell ref="A1075:T1075"/>
+    <mergeCell ref="A1064:T1064"/>
+    <mergeCell ref="D1065:E1065"/>
+    <mergeCell ref="F1065:I1065"/>
+    <mergeCell ref="J1065:L1065"/>
+    <mergeCell ref="M1065:O1065"/>
+    <mergeCell ref="P1065:R1065"/>
+    <mergeCell ref="S1065:T1065"/>
+    <mergeCell ref="A1052:T1052"/>
+    <mergeCell ref="D1053:E1053"/>
+    <mergeCell ref="F1053:I1053"/>
+    <mergeCell ref="J1053:L1053"/>
+    <mergeCell ref="M1053:O1053"/>
+    <mergeCell ref="P1053:R1053"/>
+    <mergeCell ref="S1053:T1053"/>
+    <mergeCell ref="A1107:T1107"/>
+    <mergeCell ref="D1108:E1108"/>
+    <mergeCell ref="F1108:I1108"/>
+    <mergeCell ref="J1108:L1108"/>
+    <mergeCell ref="M1108:O1108"/>
+    <mergeCell ref="P1108:R1108"/>
+    <mergeCell ref="S1108:T1108"/>
+    <mergeCell ref="A1097:T1097"/>
+    <mergeCell ref="D1098:E1098"/>
+    <mergeCell ref="F1098:I1098"/>
+    <mergeCell ref="J1098:L1098"/>
+    <mergeCell ref="M1098:O1098"/>
+    <mergeCell ref="P1098:R1098"/>
+    <mergeCell ref="S1098:T1098"/>
+    <mergeCell ref="A1086:T1086"/>
+    <mergeCell ref="D1087:E1087"/>
+    <mergeCell ref="F1087:I1087"/>
+    <mergeCell ref="J1087:L1087"/>
+    <mergeCell ref="M1087:O1087"/>
+    <mergeCell ref="P1087:R1087"/>
+    <mergeCell ref="S1087:T1087"/>
+    <mergeCell ref="A1138:T1138"/>
+    <mergeCell ref="D1139:E1139"/>
+    <mergeCell ref="F1139:I1139"/>
+    <mergeCell ref="J1139:L1139"/>
+    <mergeCell ref="M1139:O1139"/>
+    <mergeCell ref="P1139:R1139"/>
+    <mergeCell ref="S1139:T1139"/>
+    <mergeCell ref="A1128:T1128"/>
+    <mergeCell ref="D1129:E1129"/>
+    <mergeCell ref="F1129:I1129"/>
+    <mergeCell ref="J1129:L1129"/>
+    <mergeCell ref="M1129:O1129"/>
+    <mergeCell ref="P1129:R1129"/>
+    <mergeCell ref="S1129:T1129"/>
+    <mergeCell ref="A1117:T1117"/>
+    <mergeCell ref="D1118:E1118"/>
+    <mergeCell ref="F1118:I1118"/>
+    <mergeCell ref="J1118:L1118"/>
+    <mergeCell ref="M1118:O1118"/>
+    <mergeCell ref="P1118:R1118"/>
+    <mergeCell ref="S1118:T1118"/>
+    <mergeCell ref="A1171:T1171"/>
+    <mergeCell ref="D1172:E1172"/>
+    <mergeCell ref="F1172:I1172"/>
+    <mergeCell ref="J1172:L1172"/>
+    <mergeCell ref="M1172:O1172"/>
+    <mergeCell ref="P1172:R1172"/>
+    <mergeCell ref="S1172:T1172"/>
+    <mergeCell ref="A1158:T1158"/>
+    <mergeCell ref="D1159:E1159"/>
+    <mergeCell ref="F1159:I1159"/>
+    <mergeCell ref="J1159:L1159"/>
+    <mergeCell ref="M1159:O1159"/>
+    <mergeCell ref="P1159:R1159"/>
+    <mergeCell ref="S1159:T1159"/>
+    <mergeCell ref="A1148:T1148"/>
+    <mergeCell ref="D1149:E1149"/>
+    <mergeCell ref="F1149:I1149"/>
+    <mergeCell ref="J1149:L1149"/>
+    <mergeCell ref="M1149:O1149"/>
+    <mergeCell ref="P1149:R1149"/>
+    <mergeCell ref="S1149:T1149"/>
+    <mergeCell ref="A1202:T1202"/>
+    <mergeCell ref="D1203:E1203"/>
+    <mergeCell ref="F1203:I1203"/>
+    <mergeCell ref="J1203:L1203"/>
+    <mergeCell ref="M1203:O1203"/>
+    <mergeCell ref="P1203:R1203"/>
+    <mergeCell ref="S1203:T1203"/>
+    <mergeCell ref="A1201:T1201"/>
+    <mergeCell ref="A1191:T1191"/>
+    <mergeCell ref="D1192:E1192"/>
+    <mergeCell ref="F1192:I1192"/>
+    <mergeCell ref="J1192:L1192"/>
+    <mergeCell ref="M1192:O1192"/>
+    <mergeCell ref="P1192:R1192"/>
+    <mergeCell ref="S1192:T1192"/>
+    <mergeCell ref="A1181:T1181"/>
+    <mergeCell ref="D1182:E1182"/>
+    <mergeCell ref="F1182:I1182"/>
+    <mergeCell ref="J1182:L1182"/>
+    <mergeCell ref="M1182:O1182"/>
+    <mergeCell ref="P1182:R1182"/>
+    <mergeCell ref="S1182:T1182"/>
+    <mergeCell ref="A1245:T1245"/>
+    <mergeCell ref="D1246:E1246"/>
+    <mergeCell ref="F1246:I1246"/>
+    <mergeCell ref="J1246:L1246"/>
+    <mergeCell ref="M1246:O1246"/>
+    <mergeCell ref="P1246:R1246"/>
+    <mergeCell ref="S1246:T1246"/>
+    <mergeCell ref="A1231:T1231"/>
+    <mergeCell ref="D1232:E1232"/>
+    <mergeCell ref="F1232:I1232"/>
+    <mergeCell ref="J1232:L1232"/>
+    <mergeCell ref="M1232:O1232"/>
+    <mergeCell ref="P1232:R1232"/>
+    <mergeCell ref="S1232:T1232"/>
+    <mergeCell ref="A1212:T1212"/>
+    <mergeCell ref="D1213:E1213"/>
+    <mergeCell ref="F1213:I1213"/>
+    <mergeCell ref="J1213:L1213"/>
+    <mergeCell ref="M1213:O1213"/>
+    <mergeCell ref="P1213:R1213"/>
+    <mergeCell ref="S1213:T1213"/>
+    <mergeCell ref="A1288:T1288"/>
+    <mergeCell ref="D1289:E1289"/>
+    <mergeCell ref="F1289:I1289"/>
+    <mergeCell ref="J1289:L1289"/>
+    <mergeCell ref="M1289:O1289"/>
+    <mergeCell ref="P1289:R1289"/>
+    <mergeCell ref="S1289:T1289"/>
+    <mergeCell ref="A1274:T1274"/>
+    <mergeCell ref="D1275:E1275"/>
+    <mergeCell ref="F1275:I1275"/>
+    <mergeCell ref="J1275:L1275"/>
+    <mergeCell ref="M1275:O1275"/>
+    <mergeCell ref="P1275:R1275"/>
+    <mergeCell ref="S1275:T1275"/>
+    <mergeCell ref="A1255:T1255"/>
+    <mergeCell ref="D1256:E1256"/>
+    <mergeCell ref="F1256:I1256"/>
+    <mergeCell ref="J1256:L1256"/>
+    <mergeCell ref="M1256:O1256"/>
+    <mergeCell ref="P1256:R1256"/>
+    <mergeCell ref="S1256:T1256"/>
+    <mergeCell ref="A1334:T1334"/>
+    <mergeCell ref="D1335:E1335"/>
+    <mergeCell ref="F1335:I1335"/>
+    <mergeCell ref="J1335:L1335"/>
+    <mergeCell ref="M1335:O1335"/>
+    <mergeCell ref="P1335:R1335"/>
+    <mergeCell ref="S1335:T1335"/>
+    <mergeCell ref="A1314:T1314"/>
+    <mergeCell ref="D1315:E1315"/>
+    <mergeCell ref="F1315:I1315"/>
+    <mergeCell ref="J1315:L1315"/>
+    <mergeCell ref="M1315:O1315"/>
+    <mergeCell ref="P1315:R1315"/>
+    <mergeCell ref="S1315:T1315"/>
+    <mergeCell ref="A1304:T1304"/>
+    <mergeCell ref="D1305:E1305"/>
+    <mergeCell ref="F1305:I1305"/>
+    <mergeCell ref="J1305:L1305"/>
+    <mergeCell ref="M1305:O1305"/>
+    <mergeCell ref="P1305:R1305"/>
+    <mergeCell ref="S1305:T1305"/>
+    <mergeCell ref="A1374:T1374"/>
+    <mergeCell ref="D1375:E1375"/>
+    <mergeCell ref="F1375:I1375"/>
+    <mergeCell ref="J1375:L1375"/>
+    <mergeCell ref="M1375:O1375"/>
+    <mergeCell ref="P1375:R1375"/>
+    <mergeCell ref="S1375:T1375"/>
+    <mergeCell ref="A1365:T1365"/>
+    <mergeCell ref="D1366:E1366"/>
+    <mergeCell ref="F1366:I1366"/>
+    <mergeCell ref="J1366:L1366"/>
+    <mergeCell ref="M1366:O1366"/>
+    <mergeCell ref="P1366:R1366"/>
+    <mergeCell ref="S1366:T1366"/>
+    <mergeCell ref="A1348:T1348"/>
+    <mergeCell ref="D1349:E1349"/>
+    <mergeCell ref="F1349:I1349"/>
+    <mergeCell ref="J1349:L1349"/>
+    <mergeCell ref="M1349:O1349"/>
+    <mergeCell ref="P1349:R1349"/>
+    <mergeCell ref="S1349:T1349"/>
+    <mergeCell ref="A1393:T1393"/>
+    <mergeCell ref="D1394:E1394"/>
+    <mergeCell ref="F1394:I1394"/>
+    <mergeCell ref="J1394:L1394"/>
+    <mergeCell ref="M1394:O1394"/>
+    <mergeCell ref="P1394:R1394"/>
+    <mergeCell ref="S1394:T1394"/>
+    <mergeCell ref="A1388:T1388"/>
+    <mergeCell ref="D1389:E1389"/>
+    <mergeCell ref="F1389:I1389"/>
+    <mergeCell ref="J1389:L1389"/>
+    <mergeCell ref="M1389:O1389"/>
+    <mergeCell ref="P1389:R1389"/>
+    <mergeCell ref="S1389:T1389"/>
+    <mergeCell ref="A1379:T1379"/>
+    <mergeCell ref="D1380:E1380"/>
+    <mergeCell ref="F1380:I1380"/>
+    <mergeCell ref="J1380:L1380"/>
+    <mergeCell ref="M1380:O1380"/>
+    <mergeCell ref="P1380:R1380"/>
+    <mergeCell ref="S1380:T1380"/>
+    <mergeCell ref="A1420:T1420"/>
+    <mergeCell ref="D1421:E1421"/>
+    <mergeCell ref="F1421:I1421"/>
+    <mergeCell ref="J1421:L1421"/>
+    <mergeCell ref="M1421:O1421"/>
+    <mergeCell ref="P1421:R1421"/>
+    <mergeCell ref="S1421:T1421"/>
+    <mergeCell ref="A1411:T1411"/>
+    <mergeCell ref="D1412:E1412"/>
+    <mergeCell ref="F1412:I1412"/>
+    <mergeCell ref="J1412:L1412"/>
+    <mergeCell ref="M1412:O1412"/>
+    <mergeCell ref="P1412:R1412"/>
+    <mergeCell ref="S1412:T1412"/>
+    <mergeCell ref="A1402:T1402"/>
+    <mergeCell ref="D1403:E1403"/>
+    <mergeCell ref="F1403:I1403"/>
+    <mergeCell ref="J1403:L1403"/>
+    <mergeCell ref="M1403:O1403"/>
+    <mergeCell ref="P1403:R1403"/>
+    <mergeCell ref="S1403:T1403"/>
+    <mergeCell ref="A1447:T1447"/>
+    <mergeCell ref="D1448:E1448"/>
+    <mergeCell ref="F1448:I1448"/>
+    <mergeCell ref="J1448:L1448"/>
+    <mergeCell ref="M1448:O1448"/>
+    <mergeCell ref="P1448:R1448"/>
+    <mergeCell ref="S1448:T1448"/>
+    <mergeCell ref="A1438:T1438"/>
+    <mergeCell ref="D1439:E1439"/>
+    <mergeCell ref="F1439:I1439"/>
+    <mergeCell ref="J1439:L1439"/>
+    <mergeCell ref="M1439:O1439"/>
+    <mergeCell ref="P1439:R1439"/>
+    <mergeCell ref="S1439:T1439"/>
+    <mergeCell ref="A1429:T1429"/>
+    <mergeCell ref="D1430:E1430"/>
+    <mergeCell ref="F1430:I1430"/>
+    <mergeCell ref="J1430:L1430"/>
+    <mergeCell ref="M1430:O1430"/>
+    <mergeCell ref="P1430:R1430"/>
+    <mergeCell ref="S1430:T1430"/>
     <mergeCell ref="A1481:T1481"/>
     <mergeCell ref="D1482:E1482"/>
     <mergeCell ref="F1482:I1482"/>
@@ -70452,896 +71109,279 @@
     <mergeCell ref="M1457:O1457"/>
     <mergeCell ref="P1457:R1457"/>
     <mergeCell ref="S1457:T1457"/>
-    <mergeCell ref="A1447:T1447"/>
-    <mergeCell ref="D1448:E1448"/>
-    <mergeCell ref="F1448:I1448"/>
-    <mergeCell ref="J1448:L1448"/>
-    <mergeCell ref="M1448:O1448"/>
-    <mergeCell ref="P1448:R1448"/>
-    <mergeCell ref="S1448:T1448"/>
-    <mergeCell ref="A1438:T1438"/>
-    <mergeCell ref="D1439:E1439"/>
-    <mergeCell ref="F1439:I1439"/>
-    <mergeCell ref="J1439:L1439"/>
-    <mergeCell ref="M1439:O1439"/>
-    <mergeCell ref="P1439:R1439"/>
-    <mergeCell ref="S1439:T1439"/>
-    <mergeCell ref="A1429:T1429"/>
-    <mergeCell ref="D1430:E1430"/>
-    <mergeCell ref="F1430:I1430"/>
-    <mergeCell ref="J1430:L1430"/>
-    <mergeCell ref="M1430:O1430"/>
-    <mergeCell ref="P1430:R1430"/>
-    <mergeCell ref="S1430:T1430"/>
-    <mergeCell ref="A1420:T1420"/>
-    <mergeCell ref="D1421:E1421"/>
-    <mergeCell ref="F1421:I1421"/>
-    <mergeCell ref="J1421:L1421"/>
-    <mergeCell ref="M1421:O1421"/>
-    <mergeCell ref="P1421:R1421"/>
-    <mergeCell ref="S1421:T1421"/>
-    <mergeCell ref="A1411:T1411"/>
-    <mergeCell ref="D1412:E1412"/>
-    <mergeCell ref="F1412:I1412"/>
-    <mergeCell ref="J1412:L1412"/>
-    <mergeCell ref="M1412:O1412"/>
-    <mergeCell ref="P1412:R1412"/>
-    <mergeCell ref="S1412:T1412"/>
-    <mergeCell ref="A1402:T1402"/>
-    <mergeCell ref="D1403:E1403"/>
-    <mergeCell ref="F1403:I1403"/>
-    <mergeCell ref="J1403:L1403"/>
-    <mergeCell ref="M1403:O1403"/>
-    <mergeCell ref="P1403:R1403"/>
-    <mergeCell ref="S1403:T1403"/>
-    <mergeCell ref="A1393:T1393"/>
-    <mergeCell ref="D1394:E1394"/>
-    <mergeCell ref="F1394:I1394"/>
-    <mergeCell ref="J1394:L1394"/>
-    <mergeCell ref="M1394:O1394"/>
-    <mergeCell ref="P1394:R1394"/>
-    <mergeCell ref="S1394:T1394"/>
-    <mergeCell ref="A1388:T1388"/>
-    <mergeCell ref="D1389:E1389"/>
-    <mergeCell ref="F1389:I1389"/>
-    <mergeCell ref="J1389:L1389"/>
-    <mergeCell ref="M1389:O1389"/>
-    <mergeCell ref="P1389:R1389"/>
-    <mergeCell ref="S1389:T1389"/>
-    <mergeCell ref="A1379:T1379"/>
-    <mergeCell ref="D1380:E1380"/>
-    <mergeCell ref="F1380:I1380"/>
-    <mergeCell ref="J1380:L1380"/>
-    <mergeCell ref="M1380:O1380"/>
-    <mergeCell ref="P1380:R1380"/>
-    <mergeCell ref="S1380:T1380"/>
-    <mergeCell ref="A1374:T1374"/>
-    <mergeCell ref="D1375:E1375"/>
-    <mergeCell ref="F1375:I1375"/>
-    <mergeCell ref="J1375:L1375"/>
-    <mergeCell ref="M1375:O1375"/>
-    <mergeCell ref="P1375:R1375"/>
-    <mergeCell ref="S1375:T1375"/>
-    <mergeCell ref="A1365:T1365"/>
-    <mergeCell ref="D1366:E1366"/>
-    <mergeCell ref="F1366:I1366"/>
-    <mergeCell ref="J1366:L1366"/>
-    <mergeCell ref="M1366:O1366"/>
-    <mergeCell ref="P1366:R1366"/>
-    <mergeCell ref="S1366:T1366"/>
-    <mergeCell ref="A1348:T1348"/>
-    <mergeCell ref="D1349:E1349"/>
-    <mergeCell ref="F1349:I1349"/>
-    <mergeCell ref="J1349:L1349"/>
-    <mergeCell ref="M1349:O1349"/>
-    <mergeCell ref="P1349:R1349"/>
-    <mergeCell ref="S1349:T1349"/>
-    <mergeCell ref="A1334:T1334"/>
-    <mergeCell ref="D1335:E1335"/>
-    <mergeCell ref="F1335:I1335"/>
-    <mergeCell ref="J1335:L1335"/>
-    <mergeCell ref="M1335:O1335"/>
-    <mergeCell ref="P1335:R1335"/>
-    <mergeCell ref="S1335:T1335"/>
-    <mergeCell ref="A1314:T1314"/>
-    <mergeCell ref="D1315:E1315"/>
-    <mergeCell ref="F1315:I1315"/>
-    <mergeCell ref="J1315:L1315"/>
-    <mergeCell ref="M1315:O1315"/>
-    <mergeCell ref="P1315:R1315"/>
-    <mergeCell ref="S1315:T1315"/>
-    <mergeCell ref="A1304:T1304"/>
-    <mergeCell ref="D1305:E1305"/>
-    <mergeCell ref="F1305:I1305"/>
-    <mergeCell ref="J1305:L1305"/>
-    <mergeCell ref="M1305:O1305"/>
-    <mergeCell ref="P1305:R1305"/>
-    <mergeCell ref="S1305:T1305"/>
-    <mergeCell ref="A1288:T1288"/>
-    <mergeCell ref="D1289:E1289"/>
-    <mergeCell ref="F1289:I1289"/>
-    <mergeCell ref="J1289:L1289"/>
-    <mergeCell ref="M1289:O1289"/>
-    <mergeCell ref="P1289:R1289"/>
-    <mergeCell ref="S1289:T1289"/>
-    <mergeCell ref="A1274:T1274"/>
-    <mergeCell ref="D1275:E1275"/>
-    <mergeCell ref="F1275:I1275"/>
-    <mergeCell ref="J1275:L1275"/>
-    <mergeCell ref="M1275:O1275"/>
-    <mergeCell ref="P1275:R1275"/>
-    <mergeCell ref="S1275:T1275"/>
-    <mergeCell ref="A1255:T1255"/>
-    <mergeCell ref="D1256:E1256"/>
-    <mergeCell ref="F1256:I1256"/>
-    <mergeCell ref="J1256:L1256"/>
-    <mergeCell ref="M1256:O1256"/>
-    <mergeCell ref="P1256:R1256"/>
-    <mergeCell ref="S1256:T1256"/>
-    <mergeCell ref="A1245:T1245"/>
-    <mergeCell ref="D1246:E1246"/>
-    <mergeCell ref="F1246:I1246"/>
-    <mergeCell ref="J1246:L1246"/>
-    <mergeCell ref="M1246:O1246"/>
-    <mergeCell ref="P1246:R1246"/>
-    <mergeCell ref="S1246:T1246"/>
-    <mergeCell ref="A1231:T1231"/>
-    <mergeCell ref="D1232:E1232"/>
-    <mergeCell ref="F1232:I1232"/>
-    <mergeCell ref="J1232:L1232"/>
-    <mergeCell ref="M1232:O1232"/>
-    <mergeCell ref="P1232:R1232"/>
-    <mergeCell ref="S1232:T1232"/>
-    <mergeCell ref="A1212:T1212"/>
-    <mergeCell ref="D1213:E1213"/>
-    <mergeCell ref="F1213:I1213"/>
-    <mergeCell ref="J1213:L1213"/>
-    <mergeCell ref="M1213:O1213"/>
-    <mergeCell ref="P1213:R1213"/>
-    <mergeCell ref="S1213:T1213"/>
-    <mergeCell ref="A1202:T1202"/>
-    <mergeCell ref="D1203:E1203"/>
-    <mergeCell ref="F1203:I1203"/>
-    <mergeCell ref="J1203:L1203"/>
-    <mergeCell ref="M1203:O1203"/>
-    <mergeCell ref="P1203:R1203"/>
-    <mergeCell ref="S1203:T1203"/>
-    <mergeCell ref="A1201:T1201"/>
-    <mergeCell ref="A1191:T1191"/>
-    <mergeCell ref="D1192:E1192"/>
-    <mergeCell ref="F1192:I1192"/>
-    <mergeCell ref="J1192:L1192"/>
-    <mergeCell ref="M1192:O1192"/>
-    <mergeCell ref="P1192:R1192"/>
-    <mergeCell ref="S1192:T1192"/>
-    <mergeCell ref="A1181:T1181"/>
-    <mergeCell ref="D1182:E1182"/>
-    <mergeCell ref="F1182:I1182"/>
-    <mergeCell ref="J1182:L1182"/>
-    <mergeCell ref="M1182:O1182"/>
-    <mergeCell ref="P1182:R1182"/>
-    <mergeCell ref="S1182:T1182"/>
-    <mergeCell ref="A1171:T1171"/>
-    <mergeCell ref="D1172:E1172"/>
-    <mergeCell ref="F1172:I1172"/>
-    <mergeCell ref="J1172:L1172"/>
-    <mergeCell ref="M1172:O1172"/>
-    <mergeCell ref="P1172:R1172"/>
-    <mergeCell ref="S1172:T1172"/>
-    <mergeCell ref="A1158:T1158"/>
-    <mergeCell ref="D1159:E1159"/>
-    <mergeCell ref="F1159:I1159"/>
-    <mergeCell ref="J1159:L1159"/>
-    <mergeCell ref="M1159:O1159"/>
-    <mergeCell ref="P1159:R1159"/>
-    <mergeCell ref="S1159:T1159"/>
-    <mergeCell ref="A1148:T1148"/>
-    <mergeCell ref="D1149:E1149"/>
-    <mergeCell ref="F1149:I1149"/>
-    <mergeCell ref="J1149:L1149"/>
-    <mergeCell ref="M1149:O1149"/>
-    <mergeCell ref="P1149:R1149"/>
-    <mergeCell ref="S1149:T1149"/>
-    <mergeCell ref="A1138:T1138"/>
-    <mergeCell ref="D1139:E1139"/>
-    <mergeCell ref="F1139:I1139"/>
-    <mergeCell ref="J1139:L1139"/>
-    <mergeCell ref="M1139:O1139"/>
-    <mergeCell ref="P1139:R1139"/>
-    <mergeCell ref="S1139:T1139"/>
-    <mergeCell ref="A1128:T1128"/>
-    <mergeCell ref="D1129:E1129"/>
-    <mergeCell ref="F1129:I1129"/>
-    <mergeCell ref="J1129:L1129"/>
-    <mergeCell ref="M1129:O1129"/>
-    <mergeCell ref="P1129:R1129"/>
-    <mergeCell ref="S1129:T1129"/>
-    <mergeCell ref="A1117:T1117"/>
-    <mergeCell ref="D1118:E1118"/>
-    <mergeCell ref="F1118:I1118"/>
-    <mergeCell ref="J1118:L1118"/>
-    <mergeCell ref="M1118:O1118"/>
-    <mergeCell ref="P1118:R1118"/>
-    <mergeCell ref="S1118:T1118"/>
-    <mergeCell ref="A1107:T1107"/>
-    <mergeCell ref="D1108:E1108"/>
-    <mergeCell ref="F1108:I1108"/>
-    <mergeCell ref="J1108:L1108"/>
-    <mergeCell ref="M1108:O1108"/>
-    <mergeCell ref="P1108:R1108"/>
-    <mergeCell ref="S1108:T1108"/>
-    <mergeCell ref="A1097:T1097"/>
-    <mergeCell ref="D1098:E1098"/>
-    <mergeCell ref="F1098:I1098"/>
-    <mergeCell ref="J1098:L1098"/>
-    <mergeCell ref="M1098:O1098"/>
-    <mergeCell ref="P1098:R1098"/>
-    <mergeCell ref="S1098:T1098"/>
-    <mergeCell ref="A1086:T1086"/>
-    <mergeCell ref="D1087:E1087"/>
-    <mergeCell ref="F1087:I1087"/>
-    <mergeCell ref="J1087:L1087"/>
-    <mergeCell ref="M1087:O1087"/>
-    <mergeCell ref="P1087:R1087"/>
-    <mergeCell ref="S1087:T1087"/>
-    <mergeCell ref="A1076:T1076"/>
-    <mergeCell ref="D1077:E1077"/>
-    <mergeCell ref="F1077:I1077"/>
-    <mergeCell ref="J1077:L1077"/>
-    <mergeCell ref="M1077:O1077"/>
-    <mergeCell ref="P1077:R1077"/>
-    <mergeCell ref="S1077:T1077"/>
-    <mergeCell ref="A1075:T1075"/>
-    <mergeCell ref="A1064:T1064"/>
-    <mergeCell ref="D1065:E1065"/>
-    <mergeCell ref="F1065:I1065"/>
-    <mergeCell ref="J1065:L1065"/>
-    <mergeCell ref="M1065:O1065"/>
-    <mergeCell ref="P1065:R1065"/>
-    <mergeCell ref="S1065:T1065"/>
-    <mergeCell ref="A1052:T1052"/>
-    <mergeCell ref="D1053:E1053"/>
-    <mergeCell ref="F1053:I1053"/>
-    <mergeCell ref="J1053:L1053"/>
-    <mergeCell ref="M1053:O1053"/>
-    <mergeCell ref="P1053:R1053"/>
-    <mergeCell ref="S1053:T1053"/>
-    <mergeCell ref="A1041:T1041"/>
-    <mergeCell ref="D1042:E1042"/>
-    <mergeCell ref="F1042:I1042"/>
-    <mergeCell ref="J1042:L1042"/>
-    <mergeCell ref="M1042:O1042"/>
-    <mergeCell ref="P1042:R1042"/>
-    <mergeCell ref="S1042:T1042"/>
-    <mergeCell ref="A1031:T1031"/>
-    <mergeCell ref="D1032:E1032"/>
-    <mergeCell ref="F1032:I1032"/>
-    <mergeCell ref="J1032:L1032"/>
-    <mergeCell ref="M1032:O1032"/>
-    <mergeCell ref="P1032:R1032"/>
-    <mergeCell ref="S1032:T1032"/>
-    <mergeCell ref="A1017:T1017"/>
-    <mergeCell ref="D1018:E1018"/>
-    <mergeCell ref="F1018:I1018"/>
-    <mergeCell ref="J1018:L1018"/>
-    <mergeCell ref="M1018:O1018"/>
-    <mergeCell ref="P1018:R1018"/>
-    <mergeCell ref="S1018:T1018"/>
-    <mergeCell ref="A1006:T1006"/>
-    <mergeCell ref="D1007:E1007"/>
-    <mergeCell ref="F1007:I1007"/>
-    <mergeCell ref="J1007:L1007"/>
-    <mergeCell ref="M1007:O1007"/>
-    <mergeCell ref="P1007:R1007"/>
-    <mergeCell ref="S1007:T1007"/>
-    <mergeCell ref="A995:T995"/>
-    <mergeCell ref="D996:E996"/>
-    <mergeCell ref="F996:I996"/>
-    <mergeCell ref="J996:L996"/>
-    <mergeCell ref="M996:O996"/>
-    <mergeCell ref="P996:R996"/>
-    <mergeCell ref="S996:T996"/>
-    <mergeCell ref="A984:T984"/>
-    <mergeCell ref="D985:E985"/>
-    <mergeCell ref="F985:I985"/>
-    <mergeCell ref="J985:L985"/>
-    <mergeCell ref="M985:O985"/>
-    <mergeCell ref="P985:R985"/>
-    <mergeCell ref="S985:T985"/>
-    <mergeCell ref="A971:T971"/>
-    <mergeCell ref="D972:E972"/>
-    <mergeCell ref="F972:I972"/>
-    <mergeCell ref="J972:L972"/>
-    <mergeCell ref="M972:O972"/>
-    <mergeCell ref="P972:R972"/>
-    <mergeCell ref="S972:T972"/>
-    <mergeCell ref="A959:T959"/>
-    <mergeCell ref="D960:E960"/>
-    <mergeCell ref="F960:I960"/>
-    <mergeCell ref="J960:L960"/>
-    <mergeCell ref="M960:O960"/>
-    <mergeCell ref="P960:R960"/>
-    <mergeCell ref="S960:T960"/>
-    <mergeCell ref="A949:T949"/>
-    <mergeCell ref="D950:E950"/>
-    <mergeCell ref="F950:I950"/>
-    <mergeCell ref="J950:L950"/>
-    <mergeCell ref="M950:O950"/>
-    <mergeCell ref="P950:R950"/>
-    <mergeCell ref="S950:T950"/>
-    <mergeCell ref="A939:T939"/>
-    <mergeCell ref="D940:E940"/>
-    <mergeCell ref="F940:I940"/>
-    <mergeCell ref="J940:L940"/>
-    <mergeCell ref="M940:O940"/>
-    <mergeCell ref="P940:R940"/>
-    <mergeCell ref="S940:T940"/>
-    <mergeCell ref="A928:T928"/>
-    <mergeCell ref="D929:E929"/>
-    <mergeCell ref="F929:I929"/>
-    <mergeCell ref="J929:L929"/>
-    <mergeCell ref="M929:O929"/>
-    <mergeCell ref="P929:R929"/>
-    <mergeCell ref="S929:T929"/>
-    <mergeCell ref="A916:T916"/>
-    <mergeCell ref="D917:E917"/>
-    <mergeCell ref="F917:I917"/>
-    <mergeCell ref="J917:L917"/>
-    <mergeCell ref="M917:O917"/>
-    <mergeCell ref="P917:R917"/>
-    <mergeCell ref="S917:T917"/>
-    <mergeCell ref="A904:T904"/>
-    <mergeCell ref="D905:E905"/>
-    <mergeCell ref="F905:I905"/>
-    <mergeCell ref="J905:L905"/>
-    <mergeCell ref="M905:O905"/>
-    <mergeCell ref="P905:R905"/>
-    <mergeCell ref="S905:T905"/>
-    <mergeCell ref="A892:T892"/>
-    <mergeCell ref="D893:E893"/>
-    <mergeCell ref="F893:I893"/>
-    <mergeCell ref="J893:L893"/>
-    <mergeCell ref="M893:O893"/>
-    <mergeCell ref="P893:R893"/>
-    <mergeCell ref="S893:T893"/>
-    <mergeCell ref="A882:T882"/>
-    <mergeCell ref="D883:E883"/>
-    <mergeCell ref="F883:I883"/>
-    <mergeCell ref="J883:L883"/>
-    <mergeCell ref="M883:O883"/>
-    <mergeCell ref="P883:R883"/>
-    <mergeCell ref="S883:T883"/>
-    <mergeCell ref="A870:T870"/>
-    <mergeCell ref="D871:E871"/>
-    <mergeCell ref="F871:I871"/>
-    <mergeCell ref="J871:L871"/>
-    <mergeCell ref="M871:O871"/>
-    <mergeCell ref="P871:R871"/>
-    <mergeCell ref="S871:T871"/>
-    <mergeCell ref="A860:T860"/>
-    <mergeCell ref="D861:E861"/>
-    <mergeCell ref="F861:I861"/>
-    <mergeCell ref="J861:L861"/>
-    <mergeCell ref="M861:O861"/>
-    <mergeCell ref="P861:R861"/>
-    <mergeCell ref="S861:T861"/>
-    <mergeCell ref="A843:T843"/>
-    <mergeCell ref="D844:E844"/>
-    <mergeCell ref="F844:I844"/>
-    <mergeCell ref="J844:L844"/>
-    <mergeCell ref="M844:O844"/>
-    <mergeCell ref="P844:R844"/>
-    <mergeCell ref="S844:T844"/>
-    <mergeCell ref="A831:T831"/>
-    <mergeCell ref="D832:E832"/>
-    <mergeCell ref="F832:I832"/>
-    <mergeCell ref="J832:L832"/>
-    <mergeCell ref="M832:O832"/>
-    <mergeCell ref="P832:R832"/>
-    <mergeCell ref="S832:T832"/>
-    <mergeCell ref="A819:T819"/>
-    <mergeCell ref="D820:E820"/>
-    <mergeCell ref="F820:I820"/>
-    <mergeCell ref="J820:L820"/>
-    <mergeCell ref="M820:O820"/>
-    <mergeCell ref="P820:R820"/>
-    <mergeCell ref="S820:T820"/>
-    <mergeCell ref="A818:T818"/>
-    <mergeCell ref="A805:T805"/>
-    <mergeCell ref="D806:E806"/>
-    <mergeCell ref="F806:I806"/>
-    <mergeCell ref="J806:L806"/>
-    <mergeCell ref="M806:O806"/>
-    <mergeCell ref="P806:R806"/>
-    <mergeCell ref="S806:T806"/>
-    <mergeCell ref="A792:T792"/>
-    <mergeCell ref="D793:E793"/>
-    <mergeCell ref="F793:I793"/>
-    <mergeCell ref="J793:L793"/>
-    <mergeCell ref="M793:O793"/>
-    <mergeCell ref="P793:R793"/>
-    <mergeCell ref="S793:T793"/>
-    <mergeCell ref="A781:T781"/>
-    <mergeCell ref="D782:E782"/>
-    <mergeCell ref="F782:I782"/>
-    <mergeCell ref="J782:L782"/>
-    <mergeCell ref="M782:O782"/>
-    <mergeCell ref="P782:R782"/>
-    <mergeCell ref="S782:T782"/>
-    <mergeCell ref="A770:T770"/>
-    <mergeCell ref="D771:E771"/>
-    <mergeCell ref="F771:I771"/>
-    <mergeCell ref="J771:L771"/>
-    <mergeCell ref="M771:O771"/>
-    <mergeCell ref="P771:R771"/>
-    <mergeCell ref="S771:T771"/>
-    <mergeCell ref="A759:T759"/>
-    <mergeCell ref="D760:E760"/>
-    <mergeCell ref="F760:I760"/>
-    <mergeCell ref="J760:L760"/>
-    <mergeCell ref="M760:O760"/>
-    <mergeCell ref="P760:R760"/>
-    <mergeCell ref="S760:T760"/>
-    <mergeCell ref="A749:T749"/>
-    <mergeCell ref="D750:E750"/>
-    <mergeCell ref="F750:I750"/>
-    <mergeCell ref="J750:L750"/>
-    <mergeCell ref="M750:O750"/>
-    <mergeCell ref="P750:R750"/>
-    <mergeCell ref="S750:T750"/>
-    <mergeCell ref="A739:T739"/>
-    <mergeCell ref="D740:E740"/>
-    <mergeCell ref="F740:I740"/>
-    <mergeCell ref="J740:L740"/>
-    <mergeCell ref="M740:O740"/>
-    <mergeCell ref="P740:R740"/>
-    <mergeCell ref="S740:T740"/>
-    <mergeCell ref="A727:T727"/>
-    <mergeCell ref="D728:E728"/>
-    <mergeCell ref="F728:I728"/>
-    <mergeCell ref="J728:L728"/>
-    <mergeCell ref="M728:O728"/>
-    <mergeCell ref="P728:R728"/>
-    <mergeCell ref="S728:T728"/>
-    <mergeCell ref="A717:T717"/>
-    <mergeCell ref="D718:E718"/>
-    <mergeCell ref="F718:I718"/>
-    <mergeCell ref="J718:L718"/>
-    <mergeCell ref="M718:O718"/>
-    <mergeCell ref="P718:R718"/>
-    <mergeCell ref="S718:T718"/>
-    <mergeCell ref="A707:T707"/>
-    <mergeCell ref="D708:E708"/>
-    <mergeCell ref="F708:I708"/>
-    <mergeCell ref="J708:L708"/>
-    <mergeCell ref="M708:O708"/>
-    <mergeCell ref="P708:R708"/>
-    <mergeCell ref="S708:T708"/>
-    <mergeCell ref="A697:T697"/>
-    <mergeCell ref="D698:E698"/>
-    <mergeCell ref="F698:I698"/>
-    <mergeCell ref="J698:L698"/>
-    <mergeCell ref="M698:O698"/>
-    <mergeCell ref="P698:R698"/>
-    <mergeCell ref="S698:T698"/>
-    <mergeCell ref="A687:T687"/>
-    <mergeCell ref="D688:E688"/>
-    <mergeCell ref="F688:I688"/>
-    <mergeCell ref="J688:L688"/>
-    <mergeCell ref="M688:O688"/>
-    <mergeCell ref="P688:R688"/>
-    <mergeCell ref="S688:T688"/>
-    <mergeCell ref="A677:T677"/>
-    <mergeCell ref="D678:E678"/>
-    <mergeCell ref="F678:I678"/>
-    <mergeCell ref="J678:L678"/>
-    <mergeCell ref="M678:O678"/>
-    <mergeCell ref="P678:R678"/>
-    <mergeCell ref="S678:T678"/>
-    <mergeCell ref="A667:T667"/>
-    <mergeCell ref="D668:E668"/>
-    <mergeCell ref="F668:I668"/>
-    <mergeCell ref="J668:L668"/>
-    <mergeCell ref="M668:O668"/>
-    <mergeCell ref="P668:R668"/>
-    <mergeCell ref="S668:T668"/>
-    <mergeCell ref="A657:T657"/>
-    <mergeCell ref="D658:E658"/>
-    <mergeCell ref="F658:I658"/>
-    <mergeCell ref="J658:L658"/>
-    <mergeCell ref="M658:O658"/>
-    <mergeCell ref="P658:R658"/>
-    <mergeCell ref="S658:T658"/>
-    <mergeCell ref="A647:T647"/>
-    <mergeCell ref="D648:E648"/>
-    <mergeCell ref="F648:I648"/>
-    <mergeCell ref="J648:L648"/>
-    <mergeCell ref="M648:O648"/>
-    <mergeCell ref="P648:R648"/>
-    <mergeCell ref="S648:T648"/>
-    <mergeCell ref="A637:T637"/>
-    <mergeCell ref="D638:E638"/>
-    <mergeCell ref="F638:I638"/>
-    <mergeCell ref="J638:L638"/>
-    <mergeCell ref="M638:O638"/>
-    <mergeCell ref="P638:R638"/>
-    <mergeCell ref="S638:T638"/>
-    <mergeCell ref="A627:T627"/>
-    <mergeCell ref="D628:E628"/>
-    <mergeCell ref="F628:I628"/>
-    <mergeCell ref="J628:L628"/>
-    <mergeCell ref="M628:O628"/>
-    <mergeCell ref="P628:R628"/>
-    <mergeCell ref="S628:T628"/>
-    <mergeCell ref="A626:T626"/>
-    <mergeCell ref="A616:T616"/>
-    <mergeCell ref="D617:E617"/>
-    <mergeCell ref="F617:I617"/>
-    <mergeCell ref="J617:L617"/>
-    <mergeCell ref="M617:O617"/>
-    <mergeCell ref="P617:R617"/>
-    <mergeCell ref="S617:T617"/>
-    <mergeCell ref="A606:T606"/>
-    <mergeCell ref="D607:E607"/>
-    <mergeCell ref="F607:I607"/>
-    <mergeCell ref="J607:L607"/>
-    <mergeCell ref="M607:O607"/>
-    <mergeCell ref="P607:R607"/>
-    <mergeCell ref="S607:T607"/>
-    <mergeCell ref="A592:T592"/>
-    <mergeCell ref="D593:E593"/>
-    <mergeCell ref="F593:I593"/>
-    <mergeCell ref="J593:L593"/>
-    <mergeCell ref="M593:O593"/>
-    <mergeCell ref="P593:R593"/>
-    <mergeCell ref="S593:T593"/>
-    <mergeCell ref="A582:T582"/>
-    <mergeCell ref="D583:E583"/>
-    <mergeCell ref="F583:I583"/>
-    <mergeCell ref="J583:L583"/>
-    <mergeCell ref="M583:O583"/>
-    <mergeCell ref="P583:R583"/>
-    <mergeCell ref="S583:T583"/>
-    <mergeCell ref="A572:T572"/>
-    <mergeCell ref="D573:E573"/>
-    <mergeCell ref="F573:I573"/>
-    <mergeCell ref="J573:L573"/>
-    <mergeCell ref="M573:O573"/>
-    <mergeCell ref="P573:R573"/>
-    <mergeCell ref="S573:T573"/>
-    <mergeCell ref="A558:T558"/>
-    <mergeCell ref="D559:E559"/>
-    <mergeCell ref="F559:I559"/>
-    <mergeCell ref="J559:L559"/>
-    <mergeCell ref="M559:O559"/>
-    <mergeCell ref="P559:R559"/>
-    <mergeCell ref="S559:T559"/>
-    <mergeCell ref="A546:T546"/>
-    <mergeCell ref="D547:E547"/>
-    <mergeCell ref="F547:I547"/>
-    <mergeCell ref="J547:L547"/>
-    <mergeCell ref="M547:O547"/>
-    <mergeCell ref="P547:R547"/>
-    <mergeCell ref="S547:T547"/>
-    <mergeCell ref="A536:T536"/>
-    <mergeCell ref="D537:E537"/>
-    <mergeCell ref="F537:I537"/>
-    <mergeCell ref="J537:L537"/>
-    <mergeCell ref="M537:O537"/>
-    <mergeCell ref="P537:R537"/>
-    <mergeCell ref="S537:T537"/>
-    <mergeCell ref="A526:T526"/>
-    <mergeCell ref="D527:E527"/>
-    <mergeCell ref="F527:I527"/>
-    <mergeCell ref="J527:L527"/>
-    <mergeCell ref="M527:O527"/>
-    <mergeCell ref="P527:R527"/>
-    <mergeCell ref="S527:T527"/>
-    <mergeCell ref="A511:T511"/>
-    <mergeCell ref="D512:E512"/>
-    <mergeCell ref="F512:I512"/>
-    <mergeCell ref="J512:L512"/>
-    <mergeCell ref="M512:O512"/>
-    <mergeCell ref="P512:R512"/>
-    <mergeCell ref="S512:T512"/>
-    <mergeCell ref="A501:T501"/>
-    <mergeCell ref="D502:E502"/>
-    <mergeCell ref="F502:I502"/>
-    <mergeCell ref="J502:L502"/>
-    <mergeCell ref="M502:O502"/>
-    <mergeCell ref="P502:R502"/>
-    <mergeCell ref="S502:T502"/>
-    <mergeCell ref="A491:T491"/>
-    <mergeCell ref="D492:E492"/>
-    <mergeCell ref="F492:I492"/>
-    <mergeCell ref="J492:L492"/>
-    <mergeCell ref="M492:O492"/>
-    <mergeCell ref="P492:R492"/>
-    <mergeCell ref="S492:T492"/>
-    <mergeCell ref="A490:T490"/>
-    <mergeCell ref="A475:T475"/>
-    <mergeCell ref="D476:E476"/>
-    <mergeCell ref="F476:I476"/>
-    <mergeCell ref="J476:L476"/>
-    <mergeCell ref="M476:O476"/>
-    <mergeCell ref="P476:R476"/>
-    <mergeCell ref="S476:T476"/>
-    <mergeCell ref="A462:T462"/>
-    <mergeCell ref="D463:E463"/>
-    <mergeCell ref="F463:I463"/>
-    <mergeCell ref="J463:L463"/>
-    <mergeCell ref="M463:O463"/>
-    <mergeCell ref="P463:R463"/>
-    <mergeCell ref="S463:T463"/>
-    <mergeCell ref="A449:T449"/>
-    <mergeCell ref="D450:E450"/>
-    <mergeCell ref="F450:I450"/>
-    <mergeCell ref="J450:L450"/>
-    <mergeCell ref="M450:O450"/>
-    <mergeCell ref="P450:R450"/>
-    <mergeCell ref="S450:T450"/>
-    <mergeCell ref="A436:T436"/>
-    <mergeCell ref="D437:E437"/>
-    <mergeCell ref="F437:I437"/>
-    <mergeCell ref="J437:L437"/>
-    <mergeCell ref="M437:O437"/>
-    <mergeCell ref="P437:R437"/>
-    <mergeCell ref="S437:T437"/>
-    <mergeCell ref="A423:T423"/>
-    <mergeCell ref="D424:E424"/>
-    <mergeCell ref="F424:I424"/>
-    <mergeCell ref="J424:L424"/>
-    <mergeCell ref="M424:O424"/>
-    <mergeCell ref="P424:R424"/>
-    <mergeCell ref="S424:T424"/>
-    <mergeCell ref="A410:T410"/>
-    <mergeCell ref="D411:E411"/>
-    <mergeCell ref="F411:I411"/>
-    <mergeCell ref="J411:L411"/>
-    <mergeCell ref="M411:O411"/>
-    <mergeCell ref="P411:R411"/>
-    <mergeCell ref="S411:T411"/>
-    <mergeCell ref="A400:T400"/>
-    <mergeCell ref="D401:E401"/>
-    <mergeCell ref="F401:I401"/>
-    <mergeCell ref="J401:L401"/>
-    <mergeCell ref="M401:O401"/>
-    <mergeCell ref="P401:R401"/>
-    <mergeCell ref="S401:T401"/>
-    <mergeCell ref="A390:T390"/>
-    <mergeCell ref="D391:E391"/>
-    <mergeCell ref="F391:I391"/>
-    <mergeCell ref="J391:L391"/>
-    <mergeCell ref="M391:O391"/>
-    <mergeCell ref="P391:R391"/>
-    <mergeCell ref="S391:T391"/>
-    <mergeCell ref="A380:T380"/>
-    <mergeCell ref="D381:E381"/>
-    <mergeCell ref="F381:I381"/>
-    <mergeCell ref="J381:L381"/>
-    <mergeCell ref="M381:O381"/>
-    <mergeCell ref="P381:R381"/>
-    <mergeCell ref="S381:T381"/>
-    <mergeCell ref="A367:T367"/>
-    <mergeCell ref="D368:E368"/>
-    <mergeCell ref="F368:I368"/>
-    <mergeCell ref="J368:L368"/>
-    <mergeCell ref="M368:O368"/>
-    <mergeCell ref="P368:R368"/>
-    <mergeCell ref="S368:T368"/>
-    <mergeCell ref="A354:T354"/>
-    <mergeCell ref="D355:E355"/>
-    <mergeCell ref="F355:I355"/>
-    <mergeCell ref="J355:L355"/>
-    <mergeCell ref="M355:O355"/>
-    <mergeCell ref="P355:R355"/>
-    <mergeCell ref="S355:T355"/>
-    <mergeCell ref="A341:T341"/>
-    <mergeCell ref="D342:E342"/>
-    <mergeCell ref="F342:I342"/>
-    <mergeCell ref="J342:L342"/>
-    <mergeCell ref="M342:O342"/>
-    <mergeCell ref="P342:R342"/>
-    <mergeCell ref="S342:T342"/>
-    <mergeCell ref="A328:T328"/>
-    <mergeCell ref="D329:E329"/>
-    <mergeCell ref="F329:I329"/>
-    <mergeCell ref="J329:L329"/>
-    <mergeCell ref="M329:O329"/>
-    <mergeCell ref="P329:R329"/>
-    <mergeCell ref="S329:T329"/>
-    <mergeCell ref="A315:T315"/>
-    <mergeCell ref="D316:E316"/>
-    <mergeCell ref="F316:I316"/>
-    <mergeCell ref="J316:L316"/>
-    <mergeCell ref="M316:O316"/>
-    <mergeCell ref="P316:R316"/>
-    <mergeCell ref="S316:T316"/>
-    <mergeCell ref="A314:T314"/>
-    <mergeCell ref="A302:T302"/>
-    <mergeCell ref="D303:E303"/>
-    <mergeCell ref="F303:I303"/>
-    <mergeCell ref="J303:L303"/>
-    <mergeCell ref="M303:O303"/>
-    <mergeCell ref="P303:R303"/>
-    <mergeCell ref="S303:T303"/>
-    <mergeCell ref="A290:T290"/>
-    <mergeCell ref="D291:E291"/>
-    <mergeCell ref="F291:I291"/>
-    <mergeCell ref="J291:L291"/>
-    <mergeCell ref="M291:O291"/>
-    <mergeCell ref="P291:R291"/>
-    <mergeCell ref="S291:T291"/>
-    <mergeCell ref="A278:T278"/>
-    <mergeCell ref="D279:E279"/>
-    <mergeCell ref="F279:I279"/>
-    <mergeCell ref="J279:L279"/>
-    <mergeCell ref="M279:O279"/>
-    <mergeCell ref="P279:R279"/>
-    <mergeCell ref="S279:T279"/>
-    <mergeCell ref="A266:T266"/>
-    <mergeCell ref="D267:E267"/>
-    <mergeCell ref="F267:I267"/>
-    <mergeCell ref="J267:L267"/>
-    <mergeCell ref="M267:O267"/>
-    <mergeCell ref="P267:R267"/>
-    <mergeCell ref="S267:T267"/>
-    <mergeCell ref="A254:T254"/>
-    <mergeCell ref="D255:E255"/>
-    <mergeCell ref="F255:I255"/>
-    <mergeCell ref="J255:L255"/>
-    <mergeCell ref="M255:O255"/>
-    <mergeCell ref="P255:R255"/>
-    <mergeCell ref="S255:T255"/>
-    <mergeCell ref="A253:T253"/>
-    <mergeCell ref="A239:T239"/>
-    <mergeCell ref="D240:E240"/>
-    <mergeCell ref="F240:I240"/>
-    <mergeCell ref="J240:L240"/>
-    <mergeCell ref="M240:O240"/>
-    <mergeCell ref="P240:R240"/>
-    <mergeCell ref="S240:T240"/>
-    <mergeCell ref="A229:T229"/>
-    <mergeCell ref="D230:E230"/>
-    <mergeCell ref="F230:I230"/>
-    <mergeCell ref="J230:L230"/>
-    <mergeCell ref="M230:O230"/>
-    <mergeCell ref="P230:R230"/>
-    <mergeCell ref="S230:T230"/>
-    <mergeCell ref="A219:T219"/>
-    <mergeCell ref="D220:E220"/>
-    <mergeCell ref="F220:I220"/>
-    <mergeCell ref="J220:L220"/>
-    <mergeCell ref="M220:O220"/>
-    <mergeCell ref="P220:R220"/>
-    <mergeCell ref="S220:T220"/>
-    <mergeCell ref="A206:T206"/>
-    <mergeCell ref="D207:E207"/>
-    <mergeCell ref="F207:I207"/>
-    <mergeCell ref="J207:L207"/>
-    <mergeCell ref="M207:O207"/>
-    <mergeCell ref="P207:R207"/>
-    <mergeCell ref="S207:T207"/>
-    <mergeCell ref="A195:T195"/>
-    <mergeCell ref="D196:E196"/>
-    <mergeCell ref="F196:I196"/>
-    <mergeCell ref="J196:L196"/>
-    <mergeCell ref="M196:O196"/>
-    <mergeCell ref="P196:R196"/>
-    <mergeCell ref="S196:T196"/>
-    <mergeCell ref="A182:T182"/>
-    <mergeCell ref="D183:E183"/>
-    <mergeCell ref="F183:I183"/>
-    <mergeCell ref="J183:L183"/>
-    <mergeCell ref="M183:O183"/>
-    <mergeCell ref="P183:R183"/>
-    <mergeCell ref="S183:T183"/>
-    <mergeCell ref="A169:T169"/>
-    <mergeCell ref="D170:E170"/>
-    <mergeCell ref="F170:I170"/>
-    <mergeCell ref="J170:L170"/>
-    <mergeCell ref="M170:O170"/>
-    <mergeCell ref="P170:R170"/>
-    <mergeCell ref="S170:T170"/>
-    <mergeCell ref="A157:T157"/>
-    <mergeCell ref="D158:E158"/>
-    <mergeCell ref="F158:I158"/>
-    <mergeCell ref="J158:L158"/>
-    <mergeCell ref="M158:O158"/>
-    <mergeCell ref="P158:R158"/>
-    <mergeCell ref="S158:T158"/>
-    <mergeCell ref="A145:T145"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="F146:I146"/>
-    <mergeCell ref="J146:L146"/>
-    <mergeCell ref="M146:O146"/>
-    <mergeCell ref="P146:R146"/>
-    <mergeCell ref="S146:T146"/>
-    <mergeCell ref="A133:T133"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="F134:I134"/>
-    <mergeCell ref="J134:L134"/>
-    <mergeCell ref="M134:O134"/>
-    <mergeCell ref="P134:R134"/>
-    <mergeCell ref="S134:T134"/>
-    <mergeCell ref="A121:T121"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="F122:I122"/>
-    <mergeCell ref="J122:L122"/>
-    <mergeCell ref="M122:O122"/>
-    <mergeCell ref="P122:R122"/>
-    <mergeCell ref="S122:T122"/>
-    <mergeCell ref="A109:T109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="F110:I110"/>
-    <mergeCell ref="J110:L110"/>
-    <mergeCell ref="M110:O110"/>
-    <mergeCell ref="P110:R110"/>
-    <mergeCell ref="S110:T110"/>
-    <mergeCell ref="A97:T97"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="J98:L98"/>
-    <mergeCell ref="M98:O98"/>
-    <mergeCell ref="P98:R98"/>
-    <mergeCell ref="S98:T98"/>
-    <mergeCell ref="A85:T85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="F86:I86"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M86:O86"/>
-    <mergeCell ref="P86:R86"/>
-    <mergeCell ref="S86:T86"/>
-    <mergeCell ref="A73:T73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="F74:I74"/>
-    <mergeCell ref="J74:L74"/>
-    <mergeCell ref="M74:O74"/>
-    <mergeCell ref="P74:R74"/>
-    <mergeCell ref="S74:T74"/>
-    <mergeCell ref="A61:T61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="J62:L62"/>
-    <mergeCell ref="M62:O62"/>
-    <mergeCell ref="P62:R62"/>
-    <mergeCell ref="S62:T62"/>
-    <mergeCell ref="A49:T49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="J50:L50"/>
-    <mergeCell ref="M50:O50"/>
-    <mergeCell ref="P50:R50"/>
-    <mergeCell ref="S50:T50"/>
-    <mergeCell ref="A37:T37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="M38:O38"/>
-    <mergeCell ref="P38:R38"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="A25:T25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="A24:T24"/>
-    <mergeCell ref="A11:T11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="A1511:T1511"/>
+    <mergeCell ref="D1512:E1512"/>
+    <mergeCell ref="F1512:I1512"/>
+    <mergeCell ref="J1512:L1512"/>
+    <mergeCell ref="M1512:O1512"/>
+    <mergeCell ref="P1512:R1512"/>
+    <mergeCell ref="S1512:T1512"/>
+    <mergeCell ref="A1501:T1501"/>
+    <mergeCell ref="D1502:E1502"/>
+    <mergeCell ref="F1502:I1502"/>
+    <mergeCell ref="J1502:L1502"/>
+    <mergeCell ref="M1502:O1502"/>
+    <mergeCell ref="P1502:R1502"/>
+    <mergeCell ref="S1502:T1502"/>
+    <mergeCell ref="A1491:T1491"/>
+    <mergeCell ref="D1492:E1492"/>
+    <mergeCell ref="F1492:I1492"/>
+    <mergeCell ref="J1492:L1492"/>
+    <mergeCell ref="M1492:O1492"/>
+    <mergeCell ref="P1492:R1492"/>
+    <mergeCell ref="S1492:T1492"/>
+    <mergeCell ref="A1541:T1541"/>
+    <mergeCell ref="D1542:E1542"/>
+    <mergeCell ref="F1542:I1542"/>
+    <mergeCell ref="J1542:L1542"/>
+    <mergeCell ref="M1542:O1542"/>
+    <mergeCell ref="P1542:R1542"/>
+    <mergeCell ref="S1542:T1542"/>
+    <mergeCell ref="A1531:T1531"/>
+    <mergeCell ref="D1532:E1532"/>
+    <mergeCell ref="F1532:I1532"/>
+    <mergeCell ref="J1532:L1532"/>
+    <mergeCell ref="M1532:O1532"/>
+    <mergeCell ref="P1532:R1532"/>
+    <mergeCell ref="S1532:T1532"/>
+    <mergeCell ref="A1521:T1521"/>
+    <mergeCell ref="D1522:E1522"/>
+    <mergeCell ref="F1522:I1522"/>
+    <mergeCell ref="J1522:L1522"/>
+    <mergeCell ref="M1522:O1522"/>
+    <mergeCell ref="P1522:R1522"/>
+    <mergeCell ref="S1522:T1522"/>
+    <mergeCell ref="A1568:T1568"/>
+    <mergeCell ref="D1569:E1569"/>
+    <mergeCell ref="F1569:I1569"/>
+    <mergeCell ref="J1569:L1569"/>
+    <mergeCell ref="M1569:O1569"/>
+    <mergeCell ref="P1569:R1569"/>
+    <mergeCell ref="S1569:T1569"/>
+    <mergeCell ref="A1559:T1559"/>
+    <mergeCell ref="D1560:E1560"/>
+    <mergeCell ref="F1560:I1560"/>
+    <mergeCell ref="J1560:L1560"/>
+    <mergeCell ref="M1560:O1560"/>
+    <mergeCell ref="P1560:R1560"/>
+    <mergeCell ref="S1560:T1560"/>
+    <mergeCell ref="A1550:T1550"/>
+    <mergeCell ref="D1551:E1551"/>
+    <mergeCell ref="F1551:I1551"/>
+    <mergeCell ref="J1551:L1551"/>
+    <mergeCell ref="M1551:O1551"/>
+    <mergeCell ref="P1551:R1551"/>
+    <mergeCell ref="S1551:T1551"/>
+    <mergeCell ref="A1601:T1601"/>
+    <mergeCell ref="D1602:E1602"/>
+    <mergeCell ref="F1602:I1602"/>
+    <mergeCell ref="J1602:L1602"/>
+    <mergeCell ref="M1602:O1602"/>
+    <mergeCell ref="P1602:R1602"/>
+    <mergeCell ref="S1602:T1602"/>
+    <mergeCell ref="A1589:T1589"/>
+    <mergeCell ref="D1590:E1590"/>
+    <mergeCell ref="F1590:I1590"/>
+    <mergeCell ref="J1590:L1590"/>
+    <mergeCell ref="M1590:O1590"/>
+    <mergeCell ref="P1590:R1590"/>
+    <mergeCell ref="S1590:T1590"/>
+    <mergeCell ref="A1580:T1580"/>
+    <mergeCell ref="D1581:E1581"/>
+    <mergeCell ref="F1581:I1581"/>
+    <mergeCell ref="J1581:L1581"/>
+    <mergeCell ref="M1581:O1581"/>
+    <mergeCell ref="P1581:R1581"/>
+    <mergeCell ref="S1581:T1581"/>
+    <mergeCell ref="A1642:T1642"/>
+    <mergeCell ref="D1643:E1643"/>
+    <mergeCell ref="F1643:I1643"/>
+    <mergeCell ref="J1643:L1643"/>
+    <mergeCell ref="M1643:O1643"/>
+    <mergeCell ref="P1643:R1643"/>
+    <mergeCell ref="S1643:T1643"/>
+    <mergeCell ref="A1632:T1632"/>
+    <mergeCell ref="D1633:E1633"/>
+    <mergeCell ref="F1633:I1633"/>
+    <mergeCell ref="J1633:L1633"/>
+    <mergeCell ref="M1633:O1633"/>
+    <mergeCell ref="P1633:R1633"/>
+    <mergeCell ref="S1633:T1633"/>
+    <mergeCell ref="A1619:T1619"/>
+    <mergeCell ref="D1620:E1620"/>
+    <mergeCell ref="F1620:I1620"/>
+    <mergeCell ref="J1620:L1620"/>
+    <mergeCell ref="M1620:O1620"/>
+    <mergeCell ref="P1620:R1620"/>
+    <mergeCell ref="S1620:T1620"/>
+    <mergeCell ref="A1674:T1674"/>
+    <mergeCell ref="D1675:E1675"/>
+    <mergeCell ref="F1675:I1675"/>
+    <mergeCell ref="J1675:L1675"/>
+    <mergeCell ref="M1675:O1675"/>
+    <mergeCell ref="P1675:R1675"/>
+    <mergeCell ref="S1675:T1675"/>
+    <mergeCell ref="A1662:T1662"/>
+    <mergeCell ref="D1663:E1663"/>
+    <mergeCell ref="F1663:I1663"/>
+    <mergeCell ref="J1663:L1663"/>
+    <mergeCell ref="M1663:O1663"/>
+    <mergeCell ref="P1663:R1663"/>
+    <mergeCell ref="S1663:T1663"/>
+    <mergeCell ref="A1652:T1652"/>
+    <mergeCell ref="D1653:E1653"/>
+    <mergeCell ref="F1653:I1653"/>
+    <mergeCell ref="J1653:L1653"/>
+    <mergeCell ref="M1653:O1653"/>
+    <mergeCell ref="P1653:R1653"/>
+    <mergeCell ref="S1653:T1653"/>
+    <mergeCell ref="A1705:T1705"/>
+    <mergeCell ref="D1706:E1706"/>
+    <mergeCell ref="F1706:I1706"/>
+    <mergeCell ref="J1706:L1706"/>
+    <mergeCell ref="M1706:O1706"/>
+    <mergeCell ref="P1706:R1706"/>
+    <mergeCell ref="S1706:T1706"/>
+    <mergeCell ref="A1693:T1693"/>
+    <mergeCell ref="D1694:E1694"/>
+    <mergeCell ref="F1694:I1694"/>
+    <mergeCell ref="J1694:L1694"/>
+    <mergeCell ref="M1694:O1694"/>
+    <mergeCell ref="P1694:R1694"/>
+    <mergeCell ref="S1694:T1694"/>
+    <mergeCell ref="A1683:T1683"/>
+    <mergeCell ref="D1684:E1684"/>
+    <mergeCell ref="F1684:I1684"/>
+    <mergeCell ref="J1684:L1684"/>
+    <mergeCell ref="M1684:O1684"/>
+    <mergeCell ref="P1684:R1684"/>
+    <mergeCell ref="S1684:T1684"/>
+    <mergeCell ref="A1738:T1738"/>
+    <mergeCell ref="D1739:E1739"/>
+    <mergeCell ref="F1739:I1739"/>
+    <mergeCell ref="J1739:L1739"/>
+    <mergeCell ref="M1739:O1739"/>
+    <mergeCell ref="P1739:R1739"/>
+    <mergeCell ref="S1739:T1739"/>
+    <mergeCell ref="A1726:T1726"/>
+    <mergeCell ref="D1727:E1727"/>
+    <mergeCell ref="F1727:I1727"/>
+    <mergeCell ref="J1727:L1727"/>
+    <mergeCell ref="M1727:O1727"/>
+    <mergeCell ref="P1727:R1727"/>
+    <mergeCell ref="S1727:T1727"/>
+    <mergeCell ref="A1714:T1714"/>
+    <mergeCell ref="D1715:E1715"/>
+    <mergeCell ref="F1715:I1715"/>
+    <mergeCell ref="J1715:L1715"/>
+    <mergeCell ref="M1715:O1715"/>
+    <mergeCell ref="P1715:R1715"/>
+    <mergeCell ref="S1715:T1715"/>
+    <mergeCell ref="A1774:T1774"/>
+    <mergeCell ref="D1775:E1775"/>
+    <mergeCell ref="F1775:I1775"/>
+    <mergeCell ref="J1775:L1775"/>
+    <mergeCell ref="M1775:O1775"/>
+    <mergeCell ref="P1775:R1775"/>
+    <mergeCell ref="S1775:T1775"/>
+    <mergeCell ref="A1762:T1762"/>
+    <mergeCell ref="D1763:E1763"/>
+    <mergeCell ref="F1763:I1763"/>
+    <mergeCell ref="J1763:L1763"/>
+    <mergeCell ref="M1763:O1763"/>
+    <mergeCell ref="P1763:R1763"/>
+    <mergeCell ref="S1763:T1763"/>
+    <mergeCell ref="A1750:T1750"/>
+    <mergeCell ref="D1751:E1751"/>
+    <mergeCell ref="F1751:I1751"/>
+    <mergeCell ref="J1751:L1751"/>
+    <mergeCell ref="M1751:O1751"/>
+    <mergeCell ref="P1751:R1751"/>
+    <mergeCell ref="S1751:T1751"/>
+    <mergeCell ref="A1810:T1810"/>
+    <mergeCell ref="D1811:E1811"/>
+    <mergeCell ref="F1811:I1811"/>
+    <mergeCell ref="J1811:L1811"/>
+    <mergeCell ref="M1811:O1811"/>
+    <mergeCell ref="P1811:R1811"/>
+    <mergeCell ref="S1811:T1811"/>
+    <mergeCell ref="A1798:T1798"/>
+    <mergeCell ref="D1799:E1799"/>
+    <mergeCell ref="F1799:I1799"/>
+    <mergeCell ref="J1799:L1799"/>
+    <mergeCell ref="M1799:O1799"/>
+    <mergeCell ref="P1799:R1799"/>
+    <mergeCell ref="S1799:T1799"/>
+    <mergeCell ref="A1786:T1786"/>
+    <mergeCell ref="D1787:E1787"/>
+    <mergeCell ref="F1787:I1787"/>
+    <mergeCell ref="J1787:L1787"/>
+    <mergeCell ref="M1787:O1787"/>
+    <mergeCell ref="P1787:R1787"/>
+    <mergeCell ref="S1787:T1787"/>
+    <mergeCell ref="A1846:T1846"/>
+    <mergeCell ref="D1847:E1847"/>
+    <mergeCell ref="F1847:I1847"/>
+    <mergeCell ref="J1847:L1847"/>
+    <mergeCell ref="M1847:O1847"/>
+    <mergeCell ref="P1847:R1847"/>
+    <mergeCell ref="S1847:T1847"/>
+    <mergeCell ref="A1834:T1834"/>
+    <mergeCell ref="D1835:E1835"/>
+    <mergeCell ref="F1835:I1835"/>
+    <mergeCell ref="J1835:L1835"/>
+    <mergeCell ref="M1835:O1835"/>
+    <mergeCell ref="P1835:R1835"/>
+    <mergeCell ref="S1835:T1835"/>
+    <mergeCell ref="A1822:T1822"/>
+    <mergeCell ref="D1823:E1823"/>
+    <mergeCell ref="F1823:I1823"/>
+    <mergeCell ref="J1823:L1823"/>
+    <mergeCell ref="M1823:O1823"/>
+    <mergeCell ref="P1823:R1823"/>
+    <mergeCell ref="S1823:T1823"/>
+    <mergeCell ref="A1877:T1877"/>
+    <mergeCell ref="D1878:E1878"/>
+    <mergeCell ref="F1878:I1878"/>
+    <mergeCell ref="J1878:L1878"/>
+    <mergeCell ref="M1878:O1878"/>
+    <mergeCell ref="P1878:R1878"/>
+    <mergeCell ref="S1878:T1878"/>
+    <mergeCell ref="A1868:T1868"/>
+    <mergeCell ref="D1869:E1869"/>
+    <mergeCell ref="F1869:I1869"/>
+    <mergeCell ref="J1869:L1869"/>
+    <mergeCell ref="M1869:O1869"/>
+    <mergeCell ref="P1869:R1869"/>
+    <mergeCell ref="S1869:T1869"/>
+    <mergeCell ref="A1857:T1857"/>
+    <mergeCell ref="D1858:E1858"/>
+    <mergeCell ref="F1858:I1858"/>
+    <mergeCell ref="J1858:L1858"/>
+    <mergeCell ref="M1858:O1858"/>
+    <mergeCell ref="P1858:R1858"/>
+    <mergeCell ref="S1858:T1858"/>
+    <mergeCell ref="A1913:T1913"/>
+    <mergeCell ref="D1914:E1914"/>
+    <mergeCell ref="F1914:I1914"/>
+    <mergeCell ref="J1914:L1914"/>
+    <mergeCell ref="M1914:O1914"/>
+    <mergeCell ref="P1914:R1914"/>
+    <mergeCell ref="S1914:T1914"/>
+    <mergeCell ref="A1895:T1895"/>
+    <mergeCell ref="D1896:E1896"/>
+    <mergeCell ref="F1896:I1896"/>
+    <mergeCell ref="J1896:L1896"/>
+    <mergeCell ref="M1896:O1896"/>
+    <mergeCell ref="P1896:R1896"/>
+    <mergeCell ref="S1896:T1896"/>
+    <mergeCell ref="A1886:T1886"/>
+    <mergeCell ref="D1887:E1887"/>
+    <mergeCell ref="F1887:I1887"/>
+    <mergeCell ref="J1887:L1887"/>
+    <mergeCell ref="M1887:O1887"/>
+    <mergeCell ref="P1887:R1887"/>
+    <mergeCell ref="S1887:T1887"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="1.1200000000000001" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>